<commit_message>
Updated training materials for ngSwitch
</commit_message>
<xml_diff>
--- a/TOC/Course_Content_Angular14_Training.xlsx
+++ b/TOC/Course_Content_Angular14_Training.xlsx
@@ -19,7 +19,7 @@
     <t>Total Duration 30 Hours</t>
   </si>
   <si>
-    <t>Angular 10</t>
+    <t>Angular 14</t>
   </si>
   <si>
     <t>Basic</t>
@@ -34,7 +34,7 @@
     <t>Module 1 - Session - 1</t>
   </si>
   <si>
-    <t>Angular 9l Introduction</t>
+    <t>Angular 14 Introduction</t>
   </si>
   <si>
     <t>Why Angular</t>
@@ -64,7 +64,7 @@
     <t>Understanding Angular Versions</t>
   </si>
   <si>
-    <t>New Feature in A10 and latest versions</t>
+    <t>New Feature in Angular14 and latest versions</t>
   </si>
   <si>
     <t>Module 1 - Session - 2</t>
@@ -508,7 +508,7 @@
     <t>Module 3 - Session - 4</t>
   </si>
   <si>
-    <t>Angular 10 Testing</t>
+    <t>Angular 14 Testing</t>
   </si>
   <si>
     <t>Testing in Typescript</t>
@@ -526,7 +526,7 @@
     <t>Day 12</t>
   </si>
   <si>
-    <t xml:space="preserve">PWA with Angular 10 </t>
+    <t>PWA with Angular 14</t>
   </si>
   <si>
     <t>Introduction of PWA</t>
@@ -574,13 +574,13 @@
     <t>Module 4 - Session - 1</t>
   </si>
   <si>
-    <t xml:space="preserve">Angular 10 Security </t>
+    <t xml:space="preserve">Angular 14 Security </t>
   </si>
   <si>
     <t>Angular integration with Java Springboot security</t>
   </si>
   <si>
-    <t>Introduction of Angular 9  build in protections</t>
+    <t>Introduction of Angular 14  build in protections</t>
   </si>
   <si>
     <t>Preventing cross-site scripting (XSS)</t>
@@ -666,9 +666,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="25">
@@ -714,6 +714,37 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -722,7 +753,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -736,17 +767,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -754,7 +777,15 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -776,18 +807,10 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -806,33 +829,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -843,16 +844,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -891,24 +891,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -921,13 +903,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -939,7 +915,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -951,7 +951,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -963,97 +1053,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1235,6 +1235,32 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
@@ -1258,30 +1284,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -1299,26 +1301,24 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1339,134 +1339,133 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="18" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1476,15 +1475,11 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1497,12 +1492,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1835,8 +1829,8 @@
   <sheetPr/>
   <dimension ref="A1:E200"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" topLeftCell="A189" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C1"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" topLeftCell="A75" workbookViewId="0">
+      <selection activeCell="F84" sqref="F84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="26.25" outlineLevelCol="4"/>
@@ -1853,1660 +1847,1659 @@
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3"/>
-    </row>
-    <row r="2" ht="27"/>
+      <c r="C1" s="2"/>
+    </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="4"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="6" t="s">
+      <c r="A3" s="3"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="6" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="8"/>
-      <c r="C4" s="9" t="s">
+      <c r="A4" s="7"/>
+      <c r="C4" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="10"/>
+      <c r="E4" s="6"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="8"/>
-      <c r="B5" s="11" t="s">
+      <c r="A5" s="7"/>
+      <c r="B5" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="10"/>
+      <c r="E5" s="6"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="8"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="13" t="s">
+      <c r="A6" s="7"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="10"/>
+      <c r="E6" s="6"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="8"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="13" t="s">
+      <c r="A7" s="7"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="10"/>
+      <c r="E7" s="6"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="11"/>
-      <c r="C8" s="13" t="s">
+      <c r="B8" s="9"/>
+      <c r="C8" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="10"/>
+      <c r="E8" s="6"/>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="8"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="13" t="s">
+      <c r="A9" s="7"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="10"/>
+      <c r="E9" s="6"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="8"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="13" t="s">
+      <c r="A10" s="7"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="10"/>
+      <c r="E10" s="6"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="8"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="13" t="s">
+      <c r="A11" s="7"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="10"/>
+      <c r="E11" s="6"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="8"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="13" t="s">
+      <c r="A12" s="7"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E12" s="10"/>
+      <c r="E12" s="6"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="8"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="13" t="s">
+      <c r="A13" s="7"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="E13" s="10"/>
+      <c r="E13" s="6"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="8"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="13" t="s">
+      <c r="A14" s="7"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E14" s="10"/>
+      <c r="E14" s="6"/>
     </row>
     <row r="15" ht="27" spans="1:5">
-      <c r="A15" s="15"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="17" t="s">
+      <c r="A15" s="12"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="E15" s="10"/>
+      <c r="E15" s="6"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="4"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="18" t="s">
+      <c r="A16" s="3"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="E16" s="7" t="s">
+      <c r="E16" s="6" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="8"/>
-      <c r="B17" s="11" t="s">
+      <c r="A17" s="7"/>
+      <c r="B17" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="E17" s="10"/>
+      <c r="E17" s="6"/>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="8"/>
-      <c r="B18" s="11"/>
-      <c r="C18" s="13" t="s">
+      <c r="A18" s="7"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E18" s="10"/>
+      <c r="E18" s="6"/>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="8"/>
-      <c r="B19" s="11"/>
-      <c r="C19" s="13" t="s">
+      <c r="A19" s="7"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E19" s="10"/>
+      <c r="E19" s="6"/>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="8"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="13" t="s">
+      <c r="A20" s="7"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="E20" s="10"/>
+      <c r="E20" s="6"/>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="8"/>
-      <c r="B21" s="11"/>
-      <c r="C21" s="13" t="s">
+      <c r="A21" s="7"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E21" s="10"/>
+      <c r="E21" s="6"/>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="14" t="s">
+      <c r="A22" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="11"/>
-      <c r="C22" s="13" t="s">
+      <c r="B22" s="9"/>
+      <c r="C22" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="E22" s="10"/>
+      <c r="E22" s="6"/>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="8"/>
-      <c r="B23" s="11"/>
-      <c r="C23" s="13" t="s">
+      <c r="A23" s="7"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="E23" s="10"/>
+      <c r="E23" s="6"/>
     </row>
     <row r="24" spans="1:5">
-      <c r="A24" s="8"/>
-      <c r="B24" s="11"/>
-      <c r="C24" s="13" t="s">
+      <c r="A24" s="7"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="E24" s="10"/>
+      <c r="E24" s="6"/>
     </row>
     <row r="25" spans="1:5">
-      <c r="A25" s="8"/>
-      <c r="B25" s="11"/>
-      <c r="C25" s="13" t="s">
+      <c r="A25" s="7"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="E25" s="10"/>
+      <c r="E25" s="6"/>
     </row>
     <row r="26" spans="1:5">
-      <c r="A26" s="8"/>
-      <c r="B26" s="11"/>
-      <c r="C26" s="13" t="s">
+      <c r="A26" s="7"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="E26" s="10"/>
+      <c r="E26" s="6"/>
     </row>
     <row r="27" spans="1:5">
-      <c r="A27" s="8"/>
-      <c r="B27" s="11"/>
-      <c r="C27" s="13" t="s">
+      <c r="A27" s="7"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="E27" s="10"/>
+      <c r="E27" s="6"/>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="8"/>
-      <c r="B28" s="11"/>
-      <c r="C28" s="13" t="s">
+      <c r="A28" s="7"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="E28" s="10"/>
+      <c r="E28" s="6"/>
     </row>
     <row r="29" spans="1:5">
-      <c r="A29" s="8"/>
-      <c r="B29" s="11"/>
-      <c r="C29" s="13" t="s">
+      <c r="A29" s="7"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="E29" s="10"/>
+      <c r="E29" s="6"/>
     </row>
     <row r="30" spans="1:5">
-      <c r="A30" s="8"/>
-      <c r="B30" s="11"/>
-      <c r="C30" s="13" t="s">
+      <c r="A30" s="7"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="E30" s="10"/>
+      <c r="E30" s="6"/>
     </row>
     <row r="31" spans="1:5">
-      <c r="A31" s="8"/>
-      <c r="B31" s="11"/>
-      <c r="C31" s="13" t="s">
+      <c r="A31" s="7"/>
+      <c r="B31" s="9"/>
+      <c r="C31" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="E31" s="10"/>
+      <c r="E31" s="6"/>
     </row>
     <row r="32" spans="1:5">
-      <c r="A32" s="8"/>
-      <c r="B32" s="11"/>
-      <c r="C32" s="13" t="s">
+      <c r="A32" s="7"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="E32" s="10"/>
+      <c r="E32" s="6"/>
     </row>
     <row r="33" spans="1:5">
-      <c r="A33" s="8"/>
-      <c r="B33" s="11"/>
-      <c r="C33" s="13" t="s">
+      <c r="A33" s="7"/>
+      <c r="B33" s="9"/>
+      <c r="C33" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="E33" s="10"/>
+      <c r="E33" s="6"/>
     </row>
     <row r="34" spans="1:5">
-      <c r="A34" s="8"/>
-      <c r="B34" s="11"/>
-      <c r="C34" s="13" t="s">
+      <c r="A34" s="7"/>
+      <c r="B34" s="9"/>
+      <c r="C34" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="E34" s="10"/>
+      <c r="E34" s="6"/>
     </row>
     <row r="35" spans="1:5">
-      <c r="A35" s="8"/>
-      <c r="B35" s="11"/>
-      <c r="C35" s="13" t="s">
+      <c r="A35" s="7"/>
+      <c r="B35" s="9"/>
+      <c r="C35" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="E35" s="10"/>
+      <c r="E35" s="6"/>
     </row>
     <row r="36" spans="1:5">
-      <c r="A36" s="8"/>
-      <c r="B36" s="11"/>
-      <c r="C36" s="13" t="s">
+      <c r="A36" s="7"/>
+      <c r="B36" s="9"/>
+      <c r="C36" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="E36" s="10"/>
+      <c r="E36" s="6"/>
     </row>
     <row r="37" ht="27" spans="1:5">
-      <c r="A37" s="15"/>
-      <c r="B37" s="16"/>
-      <c r="C37" s="17" t="s">
+      <c r="A37" s="12"/>
+      <c r="B37" s="13"/>
+      <c r="C37" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="E37" s="10"/>
+      <c r="E37" s="6"/>
     </row>
     <row r="38" spans="1:5">
-      <c r="A38" s="4"/>
-      <c r="B38" s="5"/>
-      <c r="C38" s="19" t="s">
+      <c r="A38" s="3"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="E38" s="7" t="s">
+      <c r="E38" s="6" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:5">
-      <c r="A39" s="8"/>
-      <c r="B39" s="11" t="s">
+      <c r="A39" s="7"/>
+      <c r="B39" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C39" s="13" t="s">
+      <c r="C39" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="E39" s="10"/>
+      <c r="E39" s="6"/>
     </row>
     <row r="40" spans="1:5">
-      <c r="A40" s="14" t="s">
+      <c r="A40" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B40" s="11"/>
-      <c r="C40" s="13" t="s">
+      <c r="B40" s="9"/>
+      <c r="C40" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="E40" s="10"/>
+      <c r="E40" s="6"/>
     </row>
     <row r="41" spans="1:5">
-      <c r="A41" s="8"/>
-      <c r="B41" s="11"/>
-      <c r="C41" s="13" t="s">
+      <c r="A41" s="7"/>
+      <c r="B41" s="9"/>
+      <c r="C41" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="E41" s="10"/>
+      <c r="E41" s="6"/>
     </row>
     <row r="42" spans="1:5">
-      <c r="A42" s="8"/>
-      <c r="B42" s="11"/>
-      <c r="C42" s="13" t="s">
+      <c r="A42" s="7"/>
+      <c r="B42" s="9"/>
+      <c r="C42" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="E42" s="10"/>
+      <c r="E42" s="6"/>
     </row>
     <row r="43" ht="27" spans="1:5">
-      <c r="A43" s="15"/>
-      <c r="B43" s="16"/>
-      <c r="C43" s="17" t="s">
+      <c r="A43" s="12"/>
+      <c r="B43" s="13"/>
+      <c r="C43" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="E43" s="10"/>
+      <c r="E43" s="6"/>
     </row>
     <row r="44" spans="1:5">
-      <c r="A44" s="4"/>
-      <c r="B44" s="5"/>
-      <c r="C44" s="19" t="s">
+      <c r="A44" s="3"/>
+      <c r="B44" s="4"/>
+      <c r="C44" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="E44" s="10"/>
+      <c r="E44" s="6"/>
     </row>
     <row r="45" spans="1:5">
-      <c r="A45" s="8"/>
-      <c r="B45" s="11" t="s">
+      <c r="A45" s="7"/>
+      <c r="B45" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="C45" s="13" t="s">
+      <c r="C45" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="E45" s="10"/>
+      <c r="E45" s="6"/>
     </row>
     <row r="46" spans="1:5">
-      <c r="A46" s="8"/>
-      <c r="B46" s="11"/>
-      <c r="C46" s="13" t="s">
+      <c r="A46" s="7"/>
+      <c r="B46" s="9"/>
+      <c r="C46" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="E46" s="10"/>
+      <c r="E46" s="6"/>
     </row>
     <row r="47" spans="1:5">
-      <c r="A47" s="8"/>
-      <c r="B47" s="11"/>
-      <c r="C47" s="13" t="s">
+      <c r="A47" s="7"/>
+      <c r="B47" s="9"/>
+      <c r="C47" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="E47" s="10"/>
+      <c r="E47" s="6"/>
     </row>
     <row r="48" spans="1:5">
-      <c r="A48" s="8"/>
-      <c r="B48" s="11"/>
-      <c r="C48" s="13" t="s">
+      <c r="A48" s="7"/>
+      <c r="B48" s="9"/>
+      <c r="C48" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="E48" s="10"/>
+      <c r="E48" s="6"/>
     </row>
     <row r="49" spans="1:5">
-      <c r="A49" s="14" t="s">
+      <c r="A49" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B49" s="11"/>
-      <c r="C49" s="13" t="s">
+      <c r="B49" s="9"/>
+      <c r="C49" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="E49" s="10"/>
+      <c r="E49" s="6"/>
     </row>
     <row r="50" spans="1:5">
-      <c r="A50" s="8"/>
-      <c r="B50" s="11"/>
-      <c r="C50" s="13" t="s">
+      <c r="A50" s="7"/>
+      <c r="B50" s="9"/>
+      <c r="C50" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="E50" s="10"/>
+      <c r="E50" s="6"/>
     </row>
     <row r="51" spans="1:5">
-      <c r="A51" s="8"/>
-      <c r="B51" s="11"/>
-      <c r="C51" s="13" t="s">
+      <c r="A51" s="7"/>
+      <c r="B51" s="9"/>
+      <c r="C51" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="E51" s="10"/>
+      <c r="E51" s="6"/>
     </row>
     <row r="52" spans="1:5">
-      <c r="A52" s="8"/>
-      <c r="B52" s="11"/>
-      <c r="C52" s="13" t="s">
+      <c r="A52" s="7"/>
+      <c r="B52" s="9"/>
+      <c r="C52" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="E52" s="10"/>
+      <c r="E52" s="6"/>
     </row>
     <row r="53" spans="1:5">
-      <c r="A53" s="8"/>
-      <c r="B53" s="11"/>
-      <c r="C53" s="13" t="s">
+      <c r="A53" s="7"/>
+      <c r="B53" s="9"/>
+      <c r="C53" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="E53" s="10"/>
+      <c r="E53" s="6"/>
     </row>
     <row r="54" spans="1:5">
-      <c r="A54" s="8"/>
-      <c r="B54" s="11"/>
-      <c r="C54" s="13" t="s">
+      <c r="A54" s="7"/>
+      <c r="B54" s="9"/>
+      <c r="C54" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="E54" s="10"/>
+      <c r="E54" s="6"/>
     </row>
     <row r="55" spans="1:5">
-      <c r="A55" s="8"/>
-      <c r="B55" s="11"/>
-      <c r="C55" s="13" t="s">
+      <c r="A55" s="7"/>
+      <c r="B55" s="9"/>
+      <c r="C55" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="E55" s="10"/>
+      <c r="E55" s="6"/>
     </row>
     <row r="56" spans="1:5">
-      <c r="A56" s="8"/>
-      <c r="B56" s="11"/>
-      <c r="C56" s="13" t="s">
+      <c r="A56" s="7"/>
+      <c r="B56" s="9"/>
+      <c r="C56" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="E56" s="10"/>
+      <c r="E56" s="6"/>
     </row>
     <row r="57" ht="27" spans="1:5">
-      <c r="A57" s="15"/>
-      <c r="B57" s="16"/>
-      <c r="C57" s="17" t="s">
+      <c r="A57" s="12"/>
+      <c r="B57" s="13"/>
+      <c r="C57" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="E57" s="10"/>
+      <c r="E57" s="6"/>
     </row>
     <row r="58" spans="1:5">
-      <c r="A58" s="4"/>
-      <c r="B58" s="5"/>
-      <c r="C58" s="20" t="s">
+      <c r="A58" s="3"/>
+      <c r="B58" s="4"/>
+      <c r="C58" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="E58" s="7" t="s">
+      <c r="E58" s="6" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="59" spans="1:5">
-      <c r="A59" s="8"/>
-      <c r="B59" s="11" t="s">
+      <c r="A59" s="7"/>
+      <c r="B59" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C59" s="21" t="s">
+      <c r="C59" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="E59" s="10"/>
+      <c r="E59" s="6"/>
     </row>
     <row r="60" spans="1:5">
-      <c r="A60" s="8"/>
-      <c r="B60" s="11"/>
-      <c r="C60" s="13" t="s">
+      <c r="A60" s="7"/>
+      <c r="B60" s="9"/>
+      <c r="C60" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="E60" s="10"/>
+      <c r="E60" s="6"/>
     </row>
     <row r="61" spans="1:5">
-      <c r="A61" s="8"/>
-      <c r="B61" s="11"/>
-      <c r="C61" s="13" t="s">
+      <c r="A61" s="7"/>
+      <c r="B61" s="9"/>
+      <c r="C61" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="E61" s="10"/>
+      <c r="E61" s="6"/>
     </row>
     <row r="62" spans="1:5">
-      <c r="A62" s="8"/>
-      <c r="B62" s="11"/>
-      <c r="C62" s="13" t="s">
+      <c r="A62" s="7"/>
+      <c r="B62" s="9"/>
+      <c r="C62" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="E62" s="10"/>
+      <c r="E62" s="6"/>
     </row>
     <row r="63" spans="1:5">
-      <c r="A63" s="14" t="s">
+      <c r="A63" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="B63" s="11"/>
-      <c r="C63" s="13" t="s">
+      <c r="B63" s="9"/>
+      <c r="C63" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="E63" s="10"/>
+      <c r="E63" s="6"/>
     </row>
     <row r="64" spans="1:5">
-      <c r="A64" s="8"/>
-      <c r="B64" s="11"/>
-      <c r="C64" s="13" t="s">
+      <c r="A64" s="7"/>
+      <c r="B64" s="9"/>
+      <c r="C64" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="E64" s="10"/>
+      <c r="E64" s="6"/>
     </row>
     <row r="65" spans="1:5">
-      <c r="A65" s="8"/>
-      <c r="B65" s="11"/>
-      <c r="C65" s="13" t="s">
+      <c r="A65" s="7"/>
+      <c r="B65" s="9"/>
+      <c r="C65" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="E65" s="10"/>
+      <c r="E65" s="6"/>
     </row>
     <row r="66" spans="1:5">
-      <c r="A66" s="8"/>
-      <c r="B66" s="11"/>
-      <c r="C66" s="13" t="s">
+      <c r="A66" s="7"/>
+      <c r="B66" s="9"/>
+      <c r="C66" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="E66" s="10"/>
+      <c r="E66" s="6"/>
     </row>
     <row r="67" spans="1:5">
-      <c r="A67" s="8"/>
-      <c r="B67" s="11"/>
-      <c r="C67" s="13" t="s">
+      <c r="A67" s="7"/>
+      <c r="B67" s="9"/>
+      <c r="C67" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="E67" s="10"/>
+      <c r="E67" s="6"/>
     </row>
     <row r="68" spans="1:5">
-      <c r="A68" s="8"/>
-      <c r="B68" s="11"/>
-      <c r="C68" s="13" t="s">
+      <c r="A68" s="7"/>
+      <c r="B68" s="9"/>
+      <c r="C68" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="E68" s="10"/>
+      <c r="E68" s="6"/>
     </row>
     <row r="69" spans="1:5">
-      <c r="A69" s="8"/>
-      <c r="B69" s="11"/>
-      <c r="C69" s="13" t="s">
+      <c r="A69" s="7"/>
+      <c r="B69" s="9"/>
+      <c r="C69" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="E69" s="10"/>
+      <c r="E69" s="6"/>
     </row>
     <row r="70" spans="1:5">
-      <c r="A70" s="8"/>
-      <c r="B70" s="11"/>
-      <c r="C70" s="13" t="s">
+      <c r="A70" s="7"/>
+      <c r="B70" s="9"/>
+      <c r="C70" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="E70" s="10"/>
+      <c r="E70" s="6"/>
     </row>
     <row r="71" spans="1:5">
-      <c r="A71" s="8"/>
-      <c r="B71" s="11"/>
-      <c r="C71" s="13" t="s">
+      <c r="A71" s="7"/>
+      <c r="B71" s="9"/>
+      <c r="C71" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="E71" s="10"/>
+      <c r="E71" s="6"/>
     </row>
     <row r="72" spans="1:5">
-      <c r="A72" s="8"/>
-      <c r="B72" s="11"/>
-      <c r="C72" s="13" t="s">
+      <c r="A72" s="7"/>
+      <c r="B72" s="9"/>
+      <c r="C72" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="E72" s="10"/>
+      <c r="E72" s="6"/>
     </row>
     <row r="73" spans="1:5">
-      <c r="A73" s="8"/>
-      <c r="B73" s="11"/>
-      <c r="C73" s="13" t="s">
+      <c r="A73" s="7"/>
+      <c r="B73" s="9"/>
+      <c r="C73" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="E73" s="10"/>
+      <c r="E73" s="6"/>
     </row>
     <row r="74" spans="1:5">
-      <c r="A74" s="8"/>
-      <c r="B74" s="11"/>
-      <c r="C74" s="12" t="s">
+      <c r="A74" s="7"/>
+      <c r="B74" s="9"/>
+      <c r="C74" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="E74" s="10"/>
+      <c r="E74" s="6"/>
     </row>
     <row r="75" spans="1:5">
-      <c r="A75" s="8"/>
-      <c r="B75" s="11"/>
-      <c r="C75" s="13" t="s">
+      <c r="A75" s="7"/>
+      <c r="B75" s="9"/>
+      <c r="C75" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="E75" s="10"/>
+      <c r="E75" s="6"/>
     </row>
     <row r="76" spans="1:5">
-      <c r="A76" s="8"/>
-      <c r="B76" s="11"/>
-      <c r="C76" s="13" t="s">
+      <c r="A76" s="7"/>
+      <c r="B76" s="9"/>
+      <c r="C76" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="E76" s="10"/>
+      <c r="E76" s="6"/>
     </row>
     <row r="77" spans="1:5">
-      <c r="A77" s="8"/>
-      <c r="B77" s="11"/>
-      <c r="C77" s="13" t="s">
+      <c r="A77" s="7"/>
+      <c r="B77" s="9"/>
+      <c r="C77" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="E77" s="10"/>
+      <c r="E77" s="6"/>
     </row>
     <row r="78" spans="1:5">
-      <c r="A78" s="8"/>
-      <c r="B78" s="11"/>
-      <c r="C78" s="13" t="s">
+      <c r="A78" s="7"/>
+      <c r="B78" s="9"/>
+      <c r="C78" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="E78" s="10"/>
+      <c r="E78" s="6"/>
     </row>
     <row r="79" ht="27" spans="1:5">
-      <c r="A79" s="15"/>
-      <c r="B79" s="16"/>
-      <c r="C79" s="17" t="s">
+      <c r="A79" s="12"/>
+      <c r="B79" s="13"/>
+      <c r="C79" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="E79" s="10"/>
+      <c r="E79" s="6"/>
     </row>
     <row r="80" spans="1:5">
-      <c r="A80" s="4"/>
-      <c r="B80" s="22" t="s">
+      <c r="A80" s="3"/>
+      <c r="B80" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="C80" s="18" t="s">
+      <c r="C80" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="E80" s="10"/>
+      <c r="E80" s="6"/>
     </row>
     <row r="81" spans="1:5">
-      <c r="A81" s="8"/>
-      <c r="B81" s="11"/>
-      <c r="C81" s="13" t="s">
+      <c r="A81" s="7"/>
+      <c r="B81" s="9"/>
+      <c r="C81" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="E81" s="10"/>
+      <c r="E81" s="6"/>
     </row>
     <row r="82" spans="1:5">
-      <c r="A82" s="8"/>
-      <c r="B82" s="11"/>
-      <c r="C82" s="13" t="s">
+      <c r="A82" s="7"/>
+      <c r="B82" s="9"/>
+      <c r="C82" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="E82" s="10"/>
+      <c r="E82" s="6"/>
     </row>
     <row r="83" spans="1:5">
-      <c r="A83" s="8"/>
-      <c r="B83" s="11"/>
-      <c r="C83" s="13" t="s">
+      <c r="A83" s="7"/>
+      <c r="B83" s="9"/>
+      <c r="C83" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="E83" s="10"/>
+      <c r="E83" s="6"/>
     </row>
     <row r="84" spans="1:5">
-      <c r="A84" s="8"/>
-      <c r="B84" s="11"/>
-      <c r="C84" s="13" t="s">
+      <c r="A84" s="7"/>
+      <c r="B84" s="9"/>
+      <c r="C84" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="E84" s="10"/>
+      <c r="E84" s="6"/>
     </row>
     <row r="85" spans="1:5">
-      <c r="A85" s="8"/>
-      <c r="B85" s="11"/>
-      <c r="C85" s="13" t="s">
+      <c r="A85" s="7"/>
+      <c r="B85" s="9"/>
+      <c r="C85" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="E85" s="10"/>
+      <c r="E85" s="6"/>
     </row>
     <row r="86" spans="1:5">
-      <c r="A86" s="8"/>
-      <c r="B86" s="11"/>
-      <c r="C86" s="13" t="s">
+      <c r="A86" s="7"/>
+      <c r="B86" s="9"/>
+      <c r="C86" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="E86" s="10"/>
+      <c r="E86" s="6"/>
     </row>
     <row r="87" spans="1:5">
-      <c r="A87" s="8"/>
-      <c r="B87" s="11"/>
-      <c r="C87" s="13" t="s">
+      <c r="A87" s="7"/>
+      <c r="B87" s="9"/>
+      <c r="C87" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="E87" s="10"/>
+      <c r="E87" s="6"/>
     </row>
     <row r="88" spans="1:5">
-      <c r="A88" s="14" t="s">
+      <c r="A88" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="B88" s="11"/>
-      <c r="C88" s="13" t="s">
+      <c r="B88" s="9"/>
+      <c r="C88" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="E88" s="10"/>
+      <c r="E88" s="6"/>
     </row>
     <row r="89" spans="1:5">
-      <c r="A89" s="8"/>
-      <c r="B89" s="11"/>
-      <c r="C89" s="13" t="s">
+      <c r="A89" s="7"/>
+      <c r="B89" s="9"/>
+      <c r="C89" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="E89" s="10"/>
-    </row>
-    <row r="90" spans="1:5">
-      <c r="A90" s="8"/>
-      <c r="B90" s="11"/>
-      <c r="C90" s="13" t="s">
+      <c r="E89" s="6"/>
+    </row>
+    <row r="90" ht="52.5" spans="1:5">
+      <c r="A90" s="7"/>
+      <c r="B90" s="9"/>
+      <c r="C90" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="E90" s="10"/>
+      <c r="E90" s="6"/>
     </row>
     <row r="91" spans="1:5">
-      <c r="A91" s="8"/>
-      <c r="B91" s="11"/>
-      <c r="C91" s="13" t="s">
+      <c r="A91" s="7"/>
+      <c r="B91" s="9"/>
+      <c r="C91" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E91" s="10"/>
+      <c r="E91" s="6"/>
     </row>
     <row r="92" spans="1:5">
-      <c r="A92" s="8"/>
-      <c r="B92" s="11"/>
-      <c r="C92" s="13" t="s">
+      <c r="A92" s="7"/>
+      <c r="B92" s="9"/>
+      <c r="C92" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="E92" s="10"/>
+      <c r="E92" s="6"/>
     </row>
     <row r="93" spans="1:5">
-      <c r="A93" s="8"/>
-      <c r="B93" s="11" t="s">
+      <c r="A93" s="7"/>
+      <c r="B93" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="C93" s="12" t="s">
+      <c r="C93" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="E93" s="10"/>
+      <c r="E93" s="6"/>
     </row>
     <row r="94" spans="1:5">
-      <c r="A94" s="8"/>
-      <c r="B94" s="11"/>
-      <c r="C94" s="13" t="s">
+      <c r="A94" s="7"/>
+      <c r="B94" s="9"/>
+      <c r="C94" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="E94" s="10"/>
+      <c r="E94" s="6"/>
     </row>
     <row r="95" spans="1:5">
-      <c r="A95" s="8"/>
-      <c r="B95" s="11"/>
-      <c r="C95" s="13" t="s">
+      <c r="A95" s="7"/>
+      <c r="B95" s="9"/>
+      <c r="C95" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="E95" s="10"/>
+      <c r="E95" s="6"/>
     </row>
     <row r="96" spans="1:5">
-      <c r="A96" s="8"/>
-      <c r="B96" s="11"/>
-      <c r="C96" s="13" t="s">
+      <c r="A96" s="7"/>
+      <c r="B96" s="9"/>
+      <c r="C96" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="E96" s="10"/>
+      <c r="E96" s="6"/>
     </row>
     <row r="97" spans="1:5">
-      <c r="A97" s="14" t="s">
+      <c r="A97" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="B97" s="11"/>
-      <c r="C97" s="13" t="s">
+      <c r="B97" s="9"/>
+      <c r="C97" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="E97" s="10"/>
+      <c r="E97" s="6"/>
     </row>
     <row r="98" spans="1:5">
-      <c r="A98" s="8"/>
-      <c r="B98" s="11"/>
-      <c r="C98" s="13" t="s">
+      <c r="A98" s="7"/>
+      <c r="B98" s="9"/>
+      <c r="C98" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="E98" s="10"/>
+      <c r="E98" s="6"/>
     </row>
     <row r="99" spans="1:5">
-      <c r="A99" s="8"/>
-      <c r="B99" s="11"/>
-      <c r="C99" s="13" t="s">
+      <c r="A99" s="7"/>
+      <c r="B99" s="9"/>
+      <c r="C99" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="E99" s="10"/>
-    </row>
-    <row r="100" spans="1:5">
-      <c r="A100" s="8"/>
-      <c r="B100" s="11"/>
-      <c r="C100" s="13" t="s">
+      <c r="E99" s="6"/>
+    </row>
+    <row r="100" ht="52.5" spans="1:5">
+      <c r="A100" s="7"/>
+      <c r="B100" s="9"/>
+      <c r="C100" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="E100" s="10"/>
+      <c r="E100" s="6"/>
     </row>
     <row r="101" spans="1:5">
-      <c r="A101" s="8"/>
-      <c r="B101" s="11"/>
-      <c r="C101" s="13" t="s">
+      <c r="A101" s="7"/>
+      <c r="B101" s="9"/>
+      <c r="C101" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="E101" s="10"/>
+      <c r="E101" s="6"/>
     </row>
     <row r="102" spans="1:5">
-      <c r="A102" s="8"/>
-      <c r="B102" s="11" t="s">
+      <c r="A102" s="7"/>
+      <c r="B102" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="C102" s="12" t="s">
+      <c r="C102" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="E102" s="10"/>
+      <c r="E102" s="6"/>
     </row>
     <row r="103" spans="1:5">
-      <c r="A103" s="8"/>
-      <c r="B103" s="11"/>
-      <c r="C103" s="13" t="s">
+      <c r="A103" s="7"/>
+      <c r="B103" s="9"/>
+      <c r="C103" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="E103" s="10"/>
+      <c r="E103" s="6"/>
     </row>
     <row r="104" spans="1:5">
-      <c r="A104" s="8"/>
-      <c r="B104" s="11"/>
-      <c r="C104" s="13" t="s">
+      <c r="A104" s="7"/>
+      <c r="B104" s="9"/>
+      <c r="C104" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="E104" s="10"/>
+      <c r="E104" s="6"/>
     </row>
     <row r="105" spans="1:5">
-      <c r="A105" s="14" t="s">
+      <c r="A105" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="B105" s="11"/>
-      <c r="C105" s="13" t="s">
+      <c r="B105" s="9"/>
+      <c r="C105" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="E105" s="10"/>
+      <c r="E105" s="6"/>
     </row>
     <row r="106" spans="1:5">
-      <c r="A106" s="8"/>
-      <c r="B106" s="11"/>
-      <c r="C106" s="13" t="s">
+      <c r="A106" s="7"/>
+      <c r="B106" s="9"/>
+      <c r="C106" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="E106" s="10"/>
+      <c r="E106" s="6"/>
     </row>
     <row r="107" spans="1:5">
-      <c r="A107" s="8"/>
-      <c r="B107" s="11"/>
-      <c r="C107" s="13" t="s">
+      <c r="A107" s="7"/>
+      <c r="B107" s="9"/>
+      <c r="C107" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="E107" s="10"/>
+      <c r="E107" s="6"/>
     </row>
     <row r="108" spans="1:5">
-      <c r="A108" s="8"/>
-      <c r="B108" s="11"/>
-      <c r="C108" s="13" t="s">
+      <c r="A108" s="7"/>
+      <c r="B108" s="9"/>
+      <c r="C108" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="E108" s="10"/>
+      <c r="E108" s="6"/>
     </row>
     <row r="109" spans="1:5">
-      <c r="A109" s="8"/>
-      <c r="B109" s="11"/>
-      <c r="C109" s="13" t="s">
+      <c r="A109" s="7"/>
+      <c r="B109" s="9"/>
+      <c r="C109" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="E109" s="10"/>
+      <c r="E109" s="6"/>
     </row>
     <row r="110" ht="27" spans="1:5">
-      <c r="A110" s="15"/>
-      <c r="B110" s="16"/>
-      <c r="C110" s="17" t="s">
+      <c r="A110" s="12"/>
+      <c r="B110" s="13"/>
+      <c r="C110" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="E110" s="10"/>
+      <c r="E110" s="6"/>
     </row>
     <row r="111" spans="1:5">
-      <c r="A111" s="4"/>
-      <c r="B111" s="22" t="s">
+      <c r="A111" s="3"/>
+      <c r="B111" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="C111" s="20" t="s">
+      <c r="C111" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="E111" s="7" t="s">
+      <c r="E111" s="6" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="112" spans="1:5">
-      <c r="A112" s="8"/>
-      <c r="B112" s="11"/>
-      <c r="C112" s="12" t="s">
+      <c r="A112" s="7"/>
+      <c r="B112" s="9"/>
+      <c r="C112" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="E112" s="10"/>
+      <c r="E112" s="6"/>
     </row>
     <row r="113" spans="1:5">
-      <c r="A113" s="8"/>
-      <c r="B113" s="11"/>
-      <c r="C113" s="13" t="s">
+      <c r="A113" s="7"/>
+      <c r="B113" s="9"/>
+      <c r="C113" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="E113" s="10"/>
+      <c r="E113" s="6"/>
     </row>
     <row r="114" spans="1:5">
-      <c r="A114" s="8"/>
-      <c r="B114" s="11"/>
-      <c r="C114" s="13" t="s">
+      <c r="A114" s="7"/>
+      <c r="B114" s="9"/>
+      <c r="C114" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="E114" s="10"/>
+      <c r="E114" s="6"/>
     </row>
     <row r="115" spans="1:5">
-      <c r="A115" s="8"/>
-      <c r="B115" s="11"/>
-      <c r="C115" s="13" t="s">
+      <c r="A115" s="7"/>
+      <c r="B115" s="9"/>
+      <c r="C115" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="E115" s="10"/>
+      <c r="E115" s="6"/>
     </row>
     <row r="116" spans="1:5">
-      <c r="A116" s="14" t="s">
+      <c r="A116" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="B116" s="11"/>
-      <c r="C116" s="13" t="s">
+      <c r="B116" s="9"/>
+      <c r="C116" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="E116" s="10"/>
+      <c r="E116" s="6"/>
     </row>
     <row r="117" spans="1:5">
-      <c r="A117" s="8"/>
-      <c r="B117" s="11"/>
-      <c r="C117" s="13" t="s">
+      <c r="A117" s="7"/>
+      <c r="B117" s="9"/>
+      <c r="C117" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="E117" s="10"/>
+      <c r="E117" s="6"/>
     </row>
     <row r="118" spans="1:5">
-      <c r="A118" s="8"/>
-      <c r="B118" s="11"/>
-      <c r="C118" s="13" t="s">
+      <c r="A118" s="7"/>
+      <c r="B118" s="9"/>
+      <c r="C118" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="E118" s="10"/>
+      <c r="E118" s="6"/>
     </row>
     <row r="119" spans="1:5">
-      <c r="A119" s="8"/>
-      <c r="B119" s="11"/>
-      <c r="C119" s="13" t="s">
+      <c r="A119" s="7"/>
+      <c r="B119" s="9"/>
+      <c r="C119" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="E119" s="10"/>
+      <c r="E119" s="6"/>
     </row>
     <row r="120" spans="1:5">
-      <c r="A120" s="8"/>
-      <c r="B120" s="11"/>
-      <c r="C120" s="13" t="s">
+      <c r="A120" s="7"/>
+      <c r="B120" s="9"/>
+      <c r="C120" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="E120" s="10"/>
+      <c r="E120" s="6"/>
     </row>
     <row r="121" spans="1:5">
-      <c r="A121" s="8"/>
-      <c r="B121" s="11"/>
-      <c r="C121" s="13" t="s">
+      <c r="A121" s="7"/>
+      <c r="B121" s="9"/>
+      <c r="C121" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="E121" s="10"/>
+      <c r="E121" s="6"/>
     </row>
     <row r="122" spans="1:5">
-      <c r="A122" s="8"/>
-      <c r="B122" s="11"/>
-      <c r="C122" s="13" t="s">
+      <c r="A122" s="7"/>
+      <c r="B122" s="9"/>
+      <c r="C122" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="E122" s="10"/>
+      <c r="E122" s="6"/>
     </row>
     <row r="123" spans="1:5">
-      <c r="A123" s="8"/>
-      <c r="B123" s="11" t="s">
+      <c r="A123" s="7"/>
+      <c r="B123" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C123" s="12" t="s">
+      <c r="C123" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="E123" s="10"/>
+      <c r="E123" s="6"/>
     </row>
     <row r="124" spans="1:5">
-      <c r="A124" s="8"/>
-      <c r="B124" s="11"/>
-      <c r="C124" s="13" t="s">
+      <c r="A124" s="7"/>
+      <c r="B124" s="9"/>
+      <c r="C124" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="E124" s="10"/>
+      <c r="E124" s="6"/>
     </row>
     <row r="125" spans="1:5">
-      <c r="A125" s="8"/>
-      <c r="B125" s="11"/>
-      <c r="C125" s="13" t="s">
+      <c r="A125" s="7"/>
+      <c r="B125" s="9"/>
+      <c r="C125" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="E125" s="10"/>
+      <c r="E125" s="6"/>
     </row>
     <row r="126" spans="1:5">
-      <c r="A126" s="8"/>
-      <c r="B126" s="11"/>
-      <c r="C126" s="13" t="s">
+      <c r="A126" s="7"/>
+      <c r="B126" s="9"/>
+      <c r="C126" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="E126" s="10"/>
+      <c r="E126" s="6"/>
     </row>
     <row r="127" spans="1:5">
-      <c r="A127" s="14" t="s">
+      <c r="A127" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="B127" s="11"/>
-      <c r="C127" s="13" t="s">
+      <c r="B127" s="9"/>
+      <c r="C127" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="E127" s="10"/>
+      <c r="E127" s="6"/>
     </row>
     <row r="128" spans="1:5">
-      <c r="A128" s="8"/>
-      <c r="B128" s="11"/>
-      <c r="C128" s="13" t="s">
+      <c r="A128" s="7"/>
+      <c r="B128" s="9"/>
+      <c r="C128" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="E128" s="10"/>
+      <c r="E128" s="6"/>
     </row>
     <row r="129" spans="1:5">
-      <c r="A129" s="8"/>
-      <c r="B129" s="11"/>
-      <c r="C129" s="13" t="s">
+      <c r="A129" s="7"/>
+      <c r="B129" s="9"/>
+      <c r="C129" s="11" t="s">
         <v>138</v>
       </c>
-      <c r="E129" s="10"/>
+      <c r="E129" s="6"/>
     </row>
     <row r="130" spans="1:5">
-      <c r="A130" s="8"/>
-      <c r="B130" s="11"/>
-      <c r="C130" s="13" t="s">
+      <c r="A130" s="7"/>
+      <c r="B130" s="9"/>
+      <c r="C130" s="11" t="s">
         <v>139</v>
       </c>
-      <c r="E130" s="10"/>
+      <c r="E130" s="6"/>
     </row>
     <row r="131" spans="1:5">
-      <c r="A131" s="8"/>
-      <c r="B131" s="11"/>
-      <c r="C131" s="13" t="s">
+      <c r="A131" s="7"/>
+      <c r="B131" s="9"/>
+      <c r="C131" s="11" t="s">
         <v>140</v>
       </c>
-      <c r="E131" s="10"/>
+      <c r="E131" s="6"/>
     </row>
     <row r="132" spans="1:5">
-      <c r="A132" s="8"/>
-      <c r="B132" s="11"/>
-      <c r="C132" s="13" t="s">
+      <c r="A132" s="7"/>
+      <c r="B132" s="9"/>
+      <c r="C132" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="E132" s="10"/>
+      <c r="E132" s="6"/>
     </row>
     <row r="133" ht="27" spans="1:5">
-      <c r="A133" s="15"/>
-      <c r="B133" s="16"/>
-      <c r="C133" s="17" t="s">
+      <c r="A133" s="12"/>
+      <c r="B133" s="13"/>
+      <c r="C133" s="14" t="s">
         <v>142</v>
       </c>
-      <c r="E133" s="10"/>
+      <c r="E133" s="6"/>
     </row>
     <row r="134" spans="1:5">
-      <c r="A134" s="4"/>
-      <c r="B134" s="5"/>
-      <c r="C134" s="18" t="s">
+      <c r="A134" s="3"/>
+      <c r="B134" s="4"/>
+      <c r="C134" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="E134" s="10"/>
+      <c r="E134" s="6"/>
     </row>
     <row r="135" spans="1:5">
-      <c r="A135" s="8"/>
-      <c r="B135" s="11" t="s">
+      <c r="A135" s="7"/>
+      <c r="B135" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="C135" s="13" t="s">
+      <c r="C135" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="E135" s="10"/>
+      <c r="E135" s="6"/>
     </row>
     <row r="136" spans="1:5">
-      <c r="A136" s="8"/>
-      <c r="B136" s="11"/>
-      <c r="C136" s="13" t="s">
+      <c r="A136" s="7"/>
+      <c r="B136" s="9"/>
+      <c r="C136" s="11" t="s">
         <v>145</v>
       </c>
-      <c r="E136" s="10"/>
+      <c r="E136" s="6"/>
     </row>
     <row r="137" spans="1:5">
-      <c r="A137" s="8"/>
-      <c r="B137" s="11"/>
-      <c r="C137" s="13" t="s">
+      <c r="A137" s="7"/>
+      <c r="B137" s="9"/>
+      <c r="C137" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="E137" s="10"/>
+      <c r="E137" s="6"/>
     </row>
     <row r="138" spans="1:5">
-      <c r="A138" s="8"/>
-      <c r="B138" s="11"/>
-      <c r="C138" s="13" t="s">
+      <c r="A138" s="7"/>
+      <c r="B138" s="9"/>
+      <c r="C138" s="11" t="s">
         <v>147</v>
       </c>
-      <c r="E138" s="10"/>
+      <c r="E138" s="6"/>
     </row>
     <row r="139" spans="1:5">
-      <c r="A139" s="8"/>
-      <c r="B139" s="11"/>
-      <c r="C139" s="13" t="s">
+      <c r="A139" s="7"/>
+      <c r="B139" s="9"/>
+      <c r="C139" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="E139" s="10"/>
+      <c r="E139" s="6"/>
     </row>
     <row r="140" spans="1:5">
-      <c r="A140" s="8"/>
-      <c r="B140" s="11"/>
-      <c r="C140" s="13" t="s">
+      <c r="A140" s="7"/>
+      <c r="B140" s="9"/>
+      <c r="C140" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="E140" s="10"/>
+      <c r="E140" s="6"/>
     </row>
     <row r="141" spans="1:5">
-      <c r="A141" s="8"/>
-      <c r="B141" s="11"/>
-      <c r="C141" s="13" t="s">
+      <c r="A141" s="7"/>
+      <c r="B141" s="9"/>
+      <c r="C141" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="E141" s="10"/>
+      <c r="E141" s="6"/>
     </row>
     <row r="142" spans="1:5">
-      <c r="A142" s="14" t="s">
+      <c r="A142" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="B142" s="11"/>
-      <c r="C142" s="13" t="s">
+      <c r="B142" s="9"/>
+      <c r="C142" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="E142" s="10"/>
+      <c r="E142" s="6"/>
     </row>
     <row r="143" spans="1:5">
-      <c r="A143" s="8"/>
-      <c r="B143" s="11"/>
-      <c r="C143" s="13" t="s">
+      <c r="A143" s="7"/>
+      <c r="B143" s="9"/>
+      <c r="C143" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="E143" s="10"/>
+      <c r="E143" s="6"/>
     </row>
     <row r="144" spans="1:5">
-      <c r="A144" s="8"/>
-      <c r="B144" s="11"/>
-      <c r="C144" s="13" t="s">
+      <c r="A144" s="7"/>
+      <c r="B144" s="9"/>
+      <c r="C144" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="E144" s="10"/>
+      <c r="E144" s="6"/>
     </row>
     <row r="145" spans="1:5">
-      <c r="A145" s="8"/>
-      <c r="B145" s="11"/>
-      <c r="C145" s="13" t="s">
+      <c r="A145" s="7"/>
+      <c r="B145" s="9"/>
+      <c r="C145" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="E145" s="10"/>
+      <c r="E145" s="6"/>
     </row>
     <row r="146" spans="1:5">
-      <c r="A146" s="8"/>
-      <c r="B146" s="11"/>
-      <c r="C146" s="13" t="s">
+      <c r="A146" s="7"/>
+      <c r="B146" s="9"/>
+      <c r="C146" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="E146" s="10"/>
+      <c r="E146" s="6"/>
     </row>
     <row r="147" spans="1:5">
-      <c r="A147" s="8"/>
-      <c r="B147" s="11"/>
-      <c r="C147" s="13" t="s">
+      <c r="A147" s="7"/>
+      <c r="B147" s="9"/>
+      <c r="C147" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="E147" s="10"/>
+      <c r="E147" s="6"/>
     </row>
     <row r="148" spans="1:5">
-      <c r="A148" s="8"/>
-      <c r="B148" s="11"/>
-      <c r="C148" s="13" t="s">
+      <c r="A148" s="7"/>
+      <c r="B148" s="9"/>
+      <c r="C148" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="E148" s="10"/>
+      <c r="E148" s="6"/>
     </row>
     <row r="149" spans="1:5">
-      <c r="A149" s="8"/>
-      <c r="B149" s="11"/>
-      <c r="C149" s="13" t="s">
+      <c r="A149" s="7"/>
+      <c r="B149" s="9"/>
+      <c r="C149" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="E149" s="10"/>
+      <c r="E149" s="6"/>
     </row>
     <row r="150" spans="1:5">
-      <c r="A150" s="8"/>
-      <c r="B150" s="11"/>
-      <c r="C150" s="13" t="s">
+      <c r="A150" s="7"/>
+      <c r="B150" s="9"/>
+      <c r="C150" s="11" t="s">
         <v>160</v>
       </c>
-      <c r="E150" s="10"/>
+      <c r="E150" s="6"/>
     </row>
     <row r="151" spans="1:5">
-      <c r="A151" s="8"/>
-      <c r="B151" s="11"/>
-      <c r="C151" s="13" t="s">
+      <c r="A151" s="7"/>
+      <c r="B151" s="9"/>
+      <c r="C151" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="E151" s="10"/>
+      <c r="E151" s="6"/>
     </row>
     <row r="152" ht="27" spans="1:5">
-      <c r="A152" s="15"/>
-      <c r="B152" s="16"/>
-      <c r="C152" s="17" t="s">
+      <c r="A152" s="12"/>
+      <c r="B152" s="13"/>
+      <c r="C152" s="14" t="s">
         <v>162</v>
       </c>
-      <c r="E152" s="10"/>
+      <c r="E152" s="6"/>
     </row>
     <row r="153" spans="1:5">
-      <c r="A153" s="4"/>
-      <c r="B153" s="5"/>
-      <c r="C153" s="18" t="s">
+      <c r="A153" s="3"/>
+      <c r="B153" s="4"/>
+      <c r="C153" s="15" t="s">
         <v>163</v>
       </c>
-      <c r="E153" s="10"/>
+      <c r="E153" s="6"/>
     </row>
     <row r="154" spans="1:5">
-      <c r="A154" s="8"/>
-      <c r="B154" s="11" t="s">
+      <c r="A154" s="7"/>
+      <c r="B154" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C154" s="13" t="s">
+      <c r="C154" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="E154" s="10"/>
+      <c r="E154" s="6"/>
     </row>
     <row r="155" spans="1:5">
-      <c r="A155" s="8"/>
-      <c r="B155" s="11"/>
-      <c r="C155" s="13" t="s">
+      <c r="A155" s="7"/>
+      <c r="B155" s="9"/>
+      <c r="C155" s="11" t="s">
         <v>165</v>
       </c>
-      <c r="E155" s="10"/>
+      <c r="E155" s="6"/>
     </row>
     <row r="156" spans="1:5">
-      <c r="A156" s="8"/>
-      <c r="B156" s="11"/>
-      <c r="C156" s="13" t="s">
+      <c r="A156" s="7"/>
+      <c r="B156" s="9"/>
+      <c r="C156" s="11" t="s">
         <v>166</v>
       </c>
-      <c r="E156" s="10"/>
+      <c r="E156" s="6"/>
     </row>
     <row r="157" spans="1:5">
-      <c r="A157" s="8"/>
-      <c r="B157" s="11"/>
-      <c r="C157" s="13" t="s">
+      <c r="A157" s="7"/>
+      <c r="B157" s="9"/>
+      <c r="C157" s="11" t="s">
         <v>167</v>
       </c>
-      <c r="E157" s="10"/>
+      <c r="E157" s="6"/>
     </row>
     <row r="158" spans="1:5">
-      <c r="A158" s="8"/>
-      <c r="B158" s="11"/>
-      <c r="C158" s="13" t="s">
+      <c r="A158" s="7"/>
+      <c r="B158" s="9"/>
+      <c r="C158" s="11" t="s">
         <v>168</v>
       </c>
-      <c r="E158" s="10"/>
+      <c r="E158" s="6"/>
     </row>
     <row r="159" spans="1:5">
-      <c r="A159" s="14" t="s">
+      <c r="A159" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="B159" s="11"/>
-      <c r="C159" s="13" t="s">
+      <c r="B159" s="9"/>
+      <c r="C159" s="11" t="s">
         <v>170</v>
       </c>
-      <c r="E159" s="10"/>
+      <c r="E159" s="6"/>
     </row>
     <row r="160" spans="1:5">
-      <c r="A160" s="8"/>
-      <c r="B160" s="11"/>
-      <c r="C160" s="13" t="s">
+      <c r="A160" s="7"/>
+      <c r="B160" s="9"/>
+      <c r="C160" s="11" t="s">
         <v>171</v>
       </c>
-      <c r="E160" s="10"/>
-    </row>
-    <row r="161" spans="1:5">
-      <c r="A161" s="8"/>
-      <c r="B161" s="11"/>
-      <c r="C161" s="13" t="s">
+      <c r="E160" s="6"/>
+    </row>
+    <row r="161" ht="52.5" spans="1:5">
+      <c r="A161" s="7"/>
+      <c r="B161" s="9"/>
+      <c r="C161" s="20" t="s">
         <v>172</v>
       </c>
-      <c r="E161" s="10"/>
+      <c r="E161" s="6"/>
     </row>
     <row r="162" spans="1:5">
-      <c r="A162" s="8"/>
-      <c r="B162" s="11"/>
-      <c r="C162" s="13" t="s">
+      <c r="A162" s="7"/>
+      <c r="B162" s="9"/>
+      <c r="C162" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="E162" s="10"/>
+      <c r="E162" s="6"/>
     </row>
     <row r="163" spans="1:5">
-      <c r="A163" s="8"/>
-      <c r="B163" s="11"/>
-      <c r="C163" s="13" t="s">
+      <c r="A163" s="7"/>
+      <c r="B163" s="9"/>
+      <c r="C163" s="11" t="s">
         <v>174</v>
       </c>
-      <c r="E163" s="10"/>
+      <c r="E163" s="6"/>
     </row>
     <row r="164" spans="1:5">
-      <c r="A164" s="8"/>
-      <c r="B164" s="11"/>
-      <c r="C164" s="13" t="s">
+      <c r="A164" s="7"/>
+      <c r="B164" s="9"/>
+      <c r="C164" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="E164" s="10"/>
+      <c r="E164" s="6"/>
     </row>
     <row r="165" spans="1:5">
-      <c r="A165" s="8"/>
-      <c r="B165" s="11"/>
-      <c r="C165" s="23" t="s">
+      <c r="A165" s="7"/>
+      <c r="B165" s="9"/>
+      <c r="C165" s="21" t="s">
         <v>176</v>
       </c>
-      <c r="E165" s="10"/>
+      <c r="E165" s="6"/>
     </row>
     <row r="166" spans="1:5">
-      <c r="A166" s="8"/>
-      <c r="B166" s="11"/>
-      <c r="C166" s="23" t="s">
+      <c r="A166" s="7"/>
+      <c r="B166" s="9"/>
+      <c r="C166" s="21" t="s">
         <v>177</v>
       </c>
-      <c r="E166" s="10"/>
+      <c r="E166" s="6"/>
     </row>
     <row r="167" spans="1:5">
-      <c r="A167" s="8"/>
-      <c r="B167" s="11"/>
-      <c r="C167" s="23" t="s">
+      <c r="A167" s="7"/>
+      <c r="B167" s="9"/>
+      <c r="C167" s="21" t="s">
         <v>178</v>
       </c>
-      <c r="E167" s="10"/>
+      <c r="E167" s="6"/>
     </row>
     <row r="168" spans="1:5">
-      <c r="A168" s="8"/>
-      <c r="B168" s="11"/>
-      <c r="C168" s="23" t="s">
+      <c r="A168" s="7"/>
+      <c r="B168" s="9"/>
+      <c r="C168" s="21" t="s">
         <v>179</v>
       </c>
-      <c r="E168" s="10"/>
+      <c r="E168" s="6"/>
     </row>
     <row r="169" spans="1:5">
-      <c r="A169" s="8"/>
-      <c r="B169" s="11"/>
-      <c r="C169" s="23" t="s">
+      <c r="A169" s="7"/>
+      <c r="B169" s="9"/>
+      <c r="C169" s="21" t="s">
         <v>180</v>
       </c>
-      <c r="E169" s="10"/>
+      <c r="E169" s="6"/>
     </row>
     <row r="170" spans="1:5">
-      <c r="A170" s="8"/>
-      <c r="B170" s="11"/>
-      <c r="C170" s="24"/>
-      <c r="E170" s="10"/>
+      <c r="A170" s="7"/>
+      <c r="B170" s="9"/>
+      <c r="C170" s="21"/>
+      <c r="E170" s="6"/>
     </row>
     <row r="171" spans="1:5">
-      <c r="A171" s="8"/>
-      <c r="B171" s="11"/>
-      <c r="C171" s="23" t="s">
+      <c r="A171" s="7"/>
+      <c r="B171" s="9"/>
+      <c r="C171" s="21" t="s">
         <v>181</v>
       </c>
-      <c r="E171" s="10"/>
+      <c r="E171" s="6"/>
     </row>
     <row r="172" ht="27" spans="1:5">
-      <c r="A172" s="15"/>
-      <c r="B172" s="16"/>
-      <c r="C172" s="25" t="s">
+      <c r="A172" s="12"/>
+      <c r="B172" s="13"/>
+      <c r="C172" s="22" t="s">
         <v>182</v>
       </c>
-      <c r="E172" s="10"/>
+      <c r="E172" s="6"/>
     </row>
     <row r="173" spans="1:5">
-      <c r="A173" s="4"/>
-      <c r="B173" s="5"/>
-      <c r="C173" s="20" t="s">
+      <c r="A173" s="3"/>
+      <c r="B173" s="4"/>
+      <c r="C173" s="17" t="s">
         <v>183</v>
       </c>
-      <c r="E173" s="26" t="s">
+      <c r="E173" s="23" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="174" spans="1:5">
-      <c r="A174" s="8"/>
-      <c r="B174" s="11" t="s">
+      <c r="A174" s="7"/>
+      <c r="B174" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="C174" s="12" t="s">
+      <c r="C174" s="10" t="s">
         <v>185</v>
       </c>
-      <c r="E174" s="27"/>
+      <c r="E174" s="23"/>
     </row>
     <row r="175" spans="1:5">
-      <c r="A175" s="8"/>
-      <c r="B175" s="11"/>
-      <c r="C175" s="13" t="s">
+      <c r="A175" s="7"/>
+      <c r="B175" s="9"/>
+      <c r="C175" s="11" t="s">
         <v>186</v>
       </c>
-      <c r="E175" s="27"/>
+      <c r="E175" s="23"/>
     </row>
     <row r="176" spans="1:5">
-      <c r="A176" s="8"/>
-      <c r="B176" s="11"/>
-      <c r="C176" s="13" t="s">
+      <c r="A176" s="7"/>
+      <c r="B176" s="9"/>
+      <c r="C176" s="11" t="s">
         <v>187</v>
       </c>
-      <c r="E176" s="27"/>
+      <c r="E176" s="23"/>
     </row>
     <row r="177" spans="1:5">
-      <c r="A177" s="8"/>
-      <c r="B177" s="11"/>
-      <c r="C177" s="13" t="s">
+      <c r="A177" s="7"/>
+      <c r="B177" s="9"/>
+      <c r="C177" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="E177" s="27"/>
+      <c r="E177" s="23"/>
     </row>
     <row r="178" spans="1:5">
-      <c r="A178" s="8"/>
-      <c r="B178" s="11"/>
-      <c r="C178" s="13" t="s">
+      <c r="A178" s="7"/>
+      <c r="B178" s="9"/>
+      <c r="C178" s="11" t="s">
         <v>189</v>
       </c>
-      <c r="E178" s="27"/>
+      <c r="E178" s="23"/>
     </row>
     <row r="179" spans="1:5">
-      <c r="A179" s="14" t="s">
+      <c r="A179" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="B179" s="11"/>
-      <c r="C179" s="13" t="s">
+      <c r="B179" s="9"/>
+      <c r="C179" s="11" t="s">
         <v>191</v>
       </c>
-      <c r="E179" s="27"/>
+      <c r="E179" s="23"/>
     </row>
     <row r="180" spans="1:5">
-      <c r="A180" s="8"/>
-      <c r="B180" s="11"/>
-      <c r="C180" s="13" t="s">
+      <c r="A180" s="7"/>
+      <c r="B180" s="9"/>
+      <c r="C180" s="11" t="s">
         <v>192</v>
       </c>
-      <c r="E180" s="27"/>
+      <c r="E180" s="23"/>
     </row>
     <row r="181" spans="1:5">
-      <c r="A181" s="8"/>
-      <c r="B181" s="11"/>
-      <c r="C181" s="12" t="s">
+      <c r="A181" s="7"/>
+      <c r="B181" s="9"/>
+      <c r="C181" s="10" t="s">
         <v>193</v>
       </c>
-      <c r="E181" s="27"/>
+      <c r="E181" s="23"/>
     </row>
     <row r="182" spans="1:5">
-      <c r="A182" s="8"/>
-      <c r="B182" s="11"/>
-      <c r="C182" s="13" t="s">
+      <c r="A182" s="7"/>
+      <c r="B182" s="9"/>
+      <c r="C182" s="11" t="s">
         <v>194</v>
       </c>
-      <c r="E182" s="27"/>
-    </row>
-    <row r="183" spans="1:5">
-      <c r="A183" s="8"/>
-      <c r="B183" s="11"/>
-      <c r="C183" s="13" t="s">
+      <c r="E182" s="23"/>
+    </row>
+    <row r="183" ht="78.75" spans="1:5">
+      <c r="A183" s="7"/>
+      <c r="B183" s="9"/>
+      <c r="C183" s="20" t="s">
         <v>195</v>
       </c>
-      <c r="E183" s="27"/>
+      <c r="E183" s="23"/>
     </row>
     <row r="184" spans="1:5">
-      <c r="A184" s="8"/>
-      <c r="B184" s="11"/>
-      <c r="C184" s="13" t="s">
+      <c r="A184" s="7"/>
+      <c r="B184" s="9"/>
+      <c r="C184" s="11" t="s">
         <v>196</v>
       </c>
-      <c r="E184" s="27"/>
+      <c r="E184" s="23"/>
     </row>
     <row r="185" spans="1:5">
-      <c r="A185" s="8"/>
-      <c r="B185" s="11"/>
-      <c r="C185" s="13" t="s">
+      <c r="A185" s="7"/>
+      <c r="B185" s="9"/>
+      <c r="C185" s="11" t="s">
         <v>197</v>
       </c>
-      <c r="E185" s="27"/>
+      <c r="E185" s="23"/>
     </row>
     <row r="186" spans="1:5">
-      <c r="A186" s="8"/>
-      <c r="B186" s="11" t="s">
+      <c r="A186" s="7"/>
+      <c r="B186" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C186" s="28" t="s">
+      <c r="C186" s="24" t="s">
         <v>198</v>
       </c>
-      <c r="E186" s="27"/>
+      <c r="E186" s="23"/>
     </row>
     <row r="187" spans="1:5">
-      <c r="A187" s="8"/>
-      <c r="B187" s="11"/>
-      <c r="C187" s="29" t="s">
+      <c r="A187" s="7"/>
+      <c r="B187" s="9"/>
+      <c r="C187" s="25" t="s">
         <v>199</v>
       </c>
-      <c r="E187" s="27"/>
+      <c r="E187" s="23"/>
     </row>
     <row r="188" spans="1:5">
-      <c r="A188" s="8"/>
-      <c r="B188" s="11"/>
-      <c r="C188" s="29" t="s">
+      <c r="A188" s="7"/>
+      <c r="B188" s="9"/>
+      <c r="C188" s="25" t="s">
         <v>200</v>
       </c>
-      <c r="E188" s="27"/>
+      <c r="E188" s="23"/>
     </row>
     <row r="189" spans="1:5">
-      <c r="A189" s="8"/>
-      <c r="B189" s="11"/>
-      <c r="C189" s="30" t="s">
+      <c r="A189" s="7"/>
+      <c r="B189" s="9"/>
+      <c r="C189" s="26" t="s">
         <v>201</v>
       </c>
-      <c r="E189" s="27"/>
+      <c r="E189" s="23"/>
     </row>
     <row r="190" ht="51" spans="1:5">
-      <c r="A190" s="14" t="s">
+      <c r="A190" s="7" t="s">
         <v>202</v>
       </c>
-      <c r="B190" s="11"/>
-      <c r="C190" s="30" t="s">
+      <c r="B190" s="9"/>
+      <c r="C190" s="26" t="s">
         <v>203</v>
       </c>
-      <c r="E190" s="27"/>
+      <c r="E190" s="23"/>
     </row>
     <row r="191" spans="1:5">
-      <c r="A191" s="8"/>
-      <c r="B191" s="11"/>
-      <c r="C191" s="30" t="s">
+      <c r="A191" s="7"/>
+      <c r="B191" s="9"/>
+      <c r="C191" s="26" t="s">
         <v>204</v>
       </c>
-      <c r="E191" s="27"/>
+      <c r="E191" s="23"/>
     </row>
     <row r="192" spans="1:5">
-      <c r="A192" s="8"/>
-      <c r="B192" s="11"/>
-      <c r="C192" s="30" t="s">
+      <c r="A192" s="7"/>
+      <c r="B192" s="9"/>
+      <c r="C192" s="26" t="s">
         <v>205</v>
       </c>
-      <c r="E192" s="27"/>
+      <c r="E192" s="23"/>
     </row>
     <row r="193" spans="1:5">
-      <c r="A193" s="8"/>
-      <c r="B193" s="11"/>
-      <c r="C193" s="30" t="s">
+      <c r="A193" s="7"/>
+      <c r="B193" s="9"/>
+      <c r="C193" s="26" t="s">
         <v>206</v>
       </c>
-      <c r="E193" s="27"/>
+      <c r="E193" s="23"/>
     </row>
     <row r="194" spans="1:5">
-      <c r="A194" s="8"/>
-      <c r="B194" s="11"/>
-      <c r="C194" s="30" t="s">
+      <c r="A194" s="7"/>
+      <c r="B194" s="9"/>
+      <c r="C194" s="26" t="s">
         <v>207</v>
       </c>
-      <c r="E194" s="27"/>
+      <c r="E194" s="23"/>
     </row>
     <row r="195" spans="1:5">
-      <c r="A195" s="8"/>
-      <c r="B195" s="11"/>
-      <c r="C195" s="30" t="s">
+      <c r="A195" s="7"/>
+      <c r="B195" s="9"/>
+      <c r="C195" s="26" t="s">
         <v>208</v>
       </c>
-      <c r="E195" s="27"/>
+      <c r="E195" s="23"/>
     </row>
     <row r="196" spans="1:5">
-      <c r="A196" s="8"/>
-      <c r="B196" s="11" t="s">
+      <c r="A196" s="7"/>
+      <c r="B196" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C196" s="28" t="s">
+      <c r="C196" s="24" t="s">
         <v>209</v>
       </c>
-      <c r="E196" s="27"/>
+      <c r="E196" s="23"/>
     </row>
     <row r="197" spans="1:5">
-      <c r="A197" s="8"/>
-      <c r="B197" s="11"/>
-      <c r="C197" s="31" t="s">
+      <c r="A197" s="7"/>
+      <c r="B197" s="9"/>
+      <c r="C197" s="27" t="s">
         <v>210</v>
       </c>
-      <c r="E197" s="27"/>
+      <c r="E197" s="23"/>
     </row>
     <row r="198" spans="1:5">
-      <c r="A198" s="8"/>
-      <c r="B198" s="11"/>
-      <c r="C198" s="28" t="s">
+      <c r="A198" s="7"/>
+      <c r="B198" s="9"/>
+      <c r="C198" s="24" t="s">
         <v>211</v>
       </c>
-      <c r="E198" s="27"/>
+      <c r="E198" s="23"/>
     </row>
     <row r="199" spans="1:5">
-      <c r="A199" s="14" t="s">
+      <c r="A199" s="7" t="s">
         <v>212</v>
       </c>
-      <c r="B199" s="11"/>
-      <c r="C199" s="31" t="s">
+      <c r="B199" s="9"/>
+      <c r="C199" s="27" t="s">
         <v>213</v>
       </c>
-      <c r="E199" s="27"/>
+      <c r="E199" s="23"/>
     </row>
     <row r="200" spans="2:5">
-      <c r="B200" s="11"/>
-      <c r="C200" s="31" t="s">
+      <c r="B200" s="9"/>
+      <c r="C200" s="27" t="s">
         <v>214</v>
       </c>
-      <c r="E200" s="27"/>
+      <c r="E200" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="21">

</xml_diff>

<commit_message>
Addeded training materials for Week 2
</commit_message>
<xml_diff>
--- a/TOC/Course_Content_Angular14_Training.xlsx
+++ b/TOC/Course_Content_Angular14_Training.xlsx
@@ -666,10 +666,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -715,23 +715,8 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -753,30 +738,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -784,8 +745,23 @@
     </font>
     <font>
       <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -799,16 +775,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -822,7 +806,7 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -830,22 +814,8 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -857,8 +827,38 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -885,13 +885,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -909,115 +1041,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1029,25 +1053,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1218,32 +1224,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -1259,11 +1239,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1283,16 +1269,25 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
+      <right style="double">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
+      <top style="double">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
+      <bottom style="double">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -1315,10 +1310,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1336,134 +1342,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="18" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1486,28 +1492,31 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1829,8 +1838,8 @@
   <sheetPr/>
   <dimension ref="A1:E200"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" topLeftCell="A75" workbookViewId="0">
-      <selection activeCell="F84" sqref="F84"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="26.25" outlineLevelCol="4"/>
@@ -2207,7 +2216,7 @@
       <c r="B45" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="C45" s="11" t="s">
+      <c r="C45" s="17" t="s">
         <v>49</v>
       </c>
       <c r="E45" s="6"/>
@@ -2215,7 +2224,7 @@
     <row r="46" spans="1:5">
       <c r="A46" s="7"/>
       <c r="B46" s="9"/>
-      <c r="C46" s="11" t="s">
+      <c r="C46" s="17" t="s">
         <v>50</v>
       </c>
       <c r="E46" s="6"/>
@@ -2223,7 +2232,7 @@
     <row r="47" spans="1:5">
       <c r="A47" s="7"/>
       <c r="B47" s="9"/>
-      <c r="C47" s="11" t="s">
+      <c r="C47" s="17" t="s">
         <v>51</v>
       </c>
       <c r="E47" s="6"/>
@@ -2231,7 +2240,7 @@
     <row r="48" spans="1:5">
       <c r="A48" s="7"/>
       <c r="B48" s="9"/>
-      <c r="C48" s="11" t="s">
+      <c r="C48" s="18" t="s">
         <v>52</v>
       </c>
       <c r="E48" s="6"/>
@@ -2241,7 +2250,7 @@
         <v>53</v>
       </c>
       <c r="B49" s="9"/>
-      <c r="C49" s="11" t="s">
+      <c r="C49" s="17" t="s">
         <v>54</v>
       </c>
       <c r="E49" s="6"/>
@@ -2249,7 +2258,7 @@
     <row r="50" spans="1:5">
       <c r="A50" s="7"/>
       <c r="B50" s="9"/>
-      <c r="C50" s="11" t="s">
+      <c r="C50" s="17" t="s">
         <v>45</v>
       </c>
       <c r="E50" s="6"/>
@@ -2257,7 +2266,7 @@
     <row r="51" spans="1:5">
       <c r="A51" s="7"/>
       <c r="B51" s="9"/>
-      <c r="C51" s="11" t="s">
+      <c r="C51" s="17" t="s">
         <v>55</v>
       </c>
       <c r="E51" s="6"/>
@@ -2265,7 +2274,7 @@
     <row r="52" spans="1:5">
       <c r="A52" s="7"/>
       <c r="B52" s="9"/>
-      <c r="C52" s="11" t="s">
+      <c r="C52" s="17" t="s">
         <v>56</v>
       </c>
       <c r="E52" s="6"/>
@@ -2273,7 +2282,7 @@
     <row r="53" spans="1:5">
       <c r="A53" s="7"/>
       <c r="B53" s="9"/>
-      <c r="C53" s="11" t="s">
+      <c r="C53" s="17" t="s">
         <v>57</v>
       </c>
       <c r="E53" s="6"/>
@@ -2281,7 +2290,7 @@
     <row r="54" spans="1:5">
       <c r="A54" s="7"/>
       <c r="B54" s="9"/>
-      <c r="C54" s="11" t="s">
+      <c r="C54" s="18" t="s">
         <v>58</v>
       </c>
       <c r="E54" s="6"/>
@@ -2289,7 +2298,7 @@
     <row r="55" spans="1:5">
       <c r="A55" s="7"/>
       <c r="B55" s="9"/>
-      <c r="C55" s="11" t="s">
+      <c r="C55" s="18" t="s">
         <v>59</v>
       </c>
       <c r="E55" s="6"/>
@@ -2297,7 +2306,7 @@
     <row r="56" spans="1:5">
       <c r="A56" s="7"/>
       <c r="B56" s="9"/>
-      <c r="C56" s="11" t="s">
+      <c r="C56" s="18" t="s">
         <v>60</v>
       </c>
       <c r="E56" s="6"/>
@@ -2305,7 +2314,7 @@
     <row r="57" ht="27" spans="1:5">
       <c r="A57" s="12"/>
       <c r="B57" s="13"/>
-      <c r="C57" s="14" t="s">
+      <c r="C57" s="19" t="s">
         <v>61</v>
       </c>
       <c r="E57" s="6"/>
@@ -2313,7 +2322,7 @@
     <row r="58" spans="1:5">
       <c r="A58" s="3"/>
       <c r="B58" s="4"/>
-      <c r="C58" s="17" t="s">
+      <c r="C58" s="20" t="s">
         <v>62</v>
       </c>
       <c r="E58" s="6" t="s">
@@ -2325,7 +2334,7 @@
       <c r="B59" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C59" s="18" t="s">
+      <c r="C59" s="21" t="s">
         <v>63</v>
       </c>
       <c r="E59" s="6"/>
@@ -2333,7 +2342,7 @@
     <row r="60" spans="1:5">
       <c r="A60" s="7"/>
       <c r="B60" s="9"/>
-      <c r="C60" s="11" t="s">
+      <c r="C60" s="17" t="s">
         <v>64</v>
       </c>
       <c r="E60" s="6"/>
@@ -2341,7 +2350,7 @@
     <row r="61" spans="1:5">
       <c r="A61" s="7"/>
       <c r="B61" s="9"/>
-      <c r="C61" s="11" t="s">
+      <c r="C61" s="17" t="s">
         <v>65</v>
       </c>
       <c r="E61" s="6"/>
@@ -2349,7 +2358,7 @@
     <row r="62" spans="1:5">
       <c r="A62" s="7"/>
       <c r="B62" s="9"/>
-      <c r="C62" s="11" t="s">
+      <c r="C62" s="18" t="s">
         <v>58</v>
       </c>
       <c r="E62" s="6"/>
@@ -2359,7 +2368,7 @@
         <v>66</v>
       </c>
       <c r="B63" s="9"/>
-      <c r="C63" s="11" t="s">
+      <c r="C63" s="17" t="s">
         <v>67</v>
       </c>
       <c r="E63" s="6"/>
@@ -2367,7 +2376,7 @@
     <row r="64" spans="1:5">
       <c r="A64" s="7"/>
       <c r="B64" s="9"/>
-      <c r="C64" s="11" t="s">
+      <c r="C64" s="18" t="s">
         <v>68</v>
       </c>
       <c r="E64" s="6"/>
@@ -2375,7 +2384,7 @@
     <row r="65" spans="1:5">
       <c r="A65" s="7"/>
       <c r="B65" s="9"/>
-      <c r="C65" s="11" t="s">
+      <c r="C65" s="18" t="s">
         <v>69</v>
       </c>
       <c r="E65" s="6"/>
@@ -2383,7 +2392,7 @@
     <row r="66" spans="1:5">
       <c r="A66" s="7"/>
       <c r="B66" s="9"/>
-      <c r="C66" s="11" t="s">
+      <c r="C66" s="18" t="s">
         <v>70</v>
       </c>
       <c r="E66" s="6"/>
@@ -2391,7 +2400,7 @@
     <row r="67" spans="1:5">
       <c r="A67" s="7"/>
       <c r="B67" s="9"/>
-      <c r="C67" s="11" t="s">
+      <c r="C67" s="18" t="s">
         <v>71</v>
       </c>
       <c r="E67" s="6"/>
@@ -2399,7 +2408,7 @@
     <row r="68" spans="1:5">
       <c r="A68" s="7"/>
       <c r="B68" s="9"/>
-      <c r="C68" s="11" t="s">
+      <c r="C68" s="18" t="s">
         <v>72</v>
       </c>
       <c r="E68" s="6"/>
@@ -2407,7 +2416,7 @@
     <row r="69" spans="1:5">
       <c r="A69" s="7"/>
       <c r="B69" s="9"/>
-      <c r="C69" s="11" t="s">
+      <c r="C69" s="18" t="s">
         <v>73</v>
       </c>
       <c r="E69" s="6"/>
@@ -2415,7 +2424,7 @@
     <row r="70" spans="1:5">
       <c r="A70" s="7"/>
       <c r="B70" s="9"/>
-      <c r="C70" s="11" t="s">
+      <c r="C70" s="18" t="s">
         <v>74</v>
       </c>
       <c r="E70" s="6"/>
@@ -2423,7 +2432,7 @@
     <row r="71" spans="1:5">
       <c r="A71" s="7"/>
       <c r="B71" s="9"/>
-      <c r="C71" s="11" t="s">
+      <c r="C71" s="18" t="s">
         <v>75</v>
       </c>
       <c r="E71" s="6"/>
@@ -2431,7 +2440,7 @@
     <row r="72" spans="1:5">
       <c r="A72" s="7"/>
       <c r="B72" s="9"/>
-      <c r="C72" s="11" t="s">
+      <c r="C72" s="18" t="s">
         <v>76</v>
       </c>
       <c r="E72" s="6"/>
@@ -2439,7 +2448,7 @@
     <row r="73" spans="1:5">
       <c r="A73" s="7"/>
       <c r="B73" s="9"/>
-      <c r="C73" s="11" t="s">
+      <c r="C73" s="18" t="s">
         <v>77</v>
       </c>
       <c r="E73" s="6"/>
@@ -2455,7 +2464,7 @@
     <row r="75" spans="1:5">
       <c r="A75" s="7"/>
       <c r="B75" s="9"/>
-      <c r="C75" s="11" t="s">
+      <c r="C75" s="18" t="s">
         <v>79</v>
       </c>
       <c r="E75" s="6"/>
@@ -2463,7 +2472,7 @@
     <row r="76" spans="1:5">
       <c r="A76" s="7"/>
       <c r="B76" s="9"/>
-      <c r="C76" s="11" t="s">
+      <c r="C76" s="18" t="s">
         <v>80</v>
       </c>
       <c r="E76" s="6"/>
@@ -2471,7 +2480,7 @@
     <row r="77" spans="1:5">
       <c r="A77" s="7"/>
       <c r="B77" s="9"/>
-      <c r="C77" s="11" t="s">
+      <c r="C77" s="18" t="s">
         <v>81</v>
       </c>
       <c r="E77" s="6"/>
@@ -2479,7 +2488,7 @@
     <row r="78" spans="1:5">
       <c r="A78" s="7"/>
       <c r="B78" s="9"/>
-      <c r="C78" s="11" t="s">
+      <c r="C78" s="18" t="s">
         <v>82</v>
       </c>
       <c r="E78" s="6"/>
@@ -2487,14 +2496,14 @@
     <row r="79" ht="27" spans="1:5">
       <c r="A79" s="12"/>
       <c r="B79" s="13"/>
-      <c r="C79" s="14" t="s">
+      <c r="C79" s="19" t="s">
         <v>83</v>
       </c>
       <c r="E79" s="6"/>
     </row>
     <row r="80" spans="1:5">
       <c r="A80" s="3"/>
-      <c r="B80" s="19" t="s">
+      <c r="B80" s="22" t="s">
         <v>48</v>
       </c>
       <c r="C80" s="15" t="s">
@@ -2505,7 +2514,7 @@
     <row r="81" spans="1:5">
       <c r="A81" s="7"/>
       <c r="B81" s="9"/>
-      <c r="C81" s="11" t="s">
+      <c r="C81" s="18" t="s">
         <v>85</v>
       </c>
       <c r="E81" s="6"/>
@@ -2513,7 +2522,7 @@
     <row r="82" spans="1:5">
       <c r="A82" s="7"/>
       <c r="B82" s="9"/>
-      <c r="C82" s="11" t="s">
+      <c r="C82" s="18" t="s">
         <v>86</v>
       </c>
       <c r="E82" s="6"/>
@@ -2521,7 +2530,7 @@
     <row r="83" spans="1:5">
       <c r="A83" s="7"/>
       <c r="B83" s="9"/>
-      <c r="C83" s="11" t="s">
+      <c r="C83" s="18" t="s">
         <v>87</v>
       </c>
       <c r="E83" s="6"/>
@@ -2529,7 +2538,7 @@
     <row r="84" spans="1:5">
       <c r="A84" s="7"/>
       <c r="B84" s="9"/>
-      <c r="C84" s="11" t="s">
+      <c r="C84" s="18" t="s">
         <v>88</v>
       </c>
       <c r="E84" s="6"/>
@@ -2537,7 +2546,7 @@
     <row r="85" spans="1:5">
       <c r="A85" s="7"/>
       <c r="B85" s="9"/>
-      <c r="C85" s="11" t="s">
+      <c r="C85" s="18" t="s">
         <v>89</v>
       </c>
       <c r="E85" s="6"/>
@@ -2545,7 +2554,7 @@
     <row r="86" spans="1:5">
       <c r="A86" s="7"/>
       <c r="B86" s="9"/>
-      <c r="C86" s="11" t="s">
+      <c r="C86" s="18" t="s">
         <v>90</v>
       </c>
       <c r="E86" s="6"/>
@@ -2553,7 +2562,7 @@
     <row r="87" spans="1:5">
       <c r="A87" s="7"/>
       <c r="B87" s="9"/>
-      <c r="C87" s="11" t="s">
+      <c r="C87" s="18" t="s">
         <v>91</v>
       </c>
       <c r="E87" s="6"/>
@@ -2563,7 +2572,7 @@
         <v>92</v>
       </c>
       <c r="B88" s="9"/>
-      <c r="C88" s="11" t="s">
+      <c r="C88" s="18" t="s">
         <v>93</v>
       </c>
       <c r="E88" s="6"/>
@@ -2571,7 +2580,7 @@
     <row r="89" spans="1:5">
       <c r="A89" s="7"/>
       <c r="B89" s="9"/>
-      <c r="C89" s="11" t="s">
+      <c r="C89" s="18" t="s">
         <v>94</v>
       </c>
       <c r="E89" s="6"/>
@@ -2579,7 +2588,7 @@
     <row r="90" ht="52.5" spans="1:5">
       <c r="A90" s="7"/>
       <c r="B90" s="9"/>
-      <c r="C90" s="20" t="s">
+      <c r="C90" s="23" t="s">
         <v>95</v>
       </c>
       <c r="E90" s="6"/>
@@ -2587,7 +2596,7 @@
     <row r="91" spans="1:5">
       <c r="A91" s="7"/>
       <c r="B91" s="9"/>
-      <c r="C91" s="11" t="s">
+      <c r="C91" s="18" t="s">
         <v>96</v>
       </c>
       <c r="E91" s="6"/>
@@ -2595,7 +2604,7 @@
     <row r="92" spans="1:5">
       <c r="A92" s="7"/>
       <c r="B92" s="9"/>
-      <c r="C92" s="11" t="s">
+      <c r="C92" s="18" t="s">
         <v>97</v>
       </c>
       <c r="E92" s="6"/>
@@ -2613,7 +2622,7 @@
     <row r="94" spans="1:5">
       <c r="A94" s="7"/>
       <c r="B94" s="9"/>
-      <c r="C94" s="11" t="s">
+      <c r="C94" s="18" t="s">
         <v>99</v>
       </c>
       <c r="E94" s="6"/>
@@ -2621,7 +2630,7 @@
     <row r="95" spans="1:5">
       <c r="A95" s="7"/>
       <c r="B95" s="9"/>
-      <c r="C95" s="11" t="s">
+      <c r="C95" s="18" t="s">
         <v>100</v>
       </c>
       <c r="E95" s="6"/>
@@ -2629,7 +2638,7 @@
     <row r="96" spans="1:5">
       <c r="A96" s="7"/>
       <c r="B96" s="9"/>
-      <c r="C96" s="11" t="s">
+      <c r="C96" s="18" t="s">
         <v>101</v>
       </c>
       <c r="E96" s="6"/>
@@ -2639,7 +2648,7 @@
         <v>102</v>
       </c>
       <c r="B97" s="9"/>
-      <c r="C97" s="11" t="s">
+      <c r="C97" s="18" t="s">
         <v>103</v>
       </c>
       <c r="E97" s="6"/>
@@ -2647,7 +2656,7 @@
     <row r="98" spans="1:5">
       <c r="A98" s="7"/>
       <c r="B98" s="9"/>
-      <c r="C98" s="11" t="s">
+      <c r="C98" s="18" t="s">
         <v>104</v>
       </c>
       <c r="E98" s="6"/>
@@ -2655,7 +2664,7 @@
     <row r="99" spans="1:5">
       <c r="A99" s="7"/>
       <c r="B99" s="9"/>
-      <c r="C99" s="11" t="s">
+      <c r="C99" s="18" t="s">
         <v>105</v>
       </c>
       <c r="E99" s="6"/>
@@ -2663,7 +2672,7 @@
     <row r="100" ht="52.5" spans="1:5">
       <c r="A100" s="7"/>
       <c r="B100" s="9"/>
-      <c r="C100" s="20" t="s">
+      <c r="C100" s="23" t="s">
         <v>106</v>
       </c>
       <c r="E100" s="6"/>
@@ -2671,7 +2680,7 @@
     <row r="101" spans="1:5">
       <c r="A101" s="7"/>
       <c r="B101" s="9"/>
-      <c r="C101" s="11" t="s">
+      <c r="C101" s="18" t="s">
         <v>107</v>
       </c>
       <c r="E101" s="6"/>
@@ -2689,7 +2698,7 @@
     <row r="103" spans="1:5">
       <c r="A103" s="7"/>
       <c r="B103" s="9"/>
-      <c r="C103" s="11" t="s">
+      <c r="C103" s="18" t="s">
         <v>109</v>
       </c>
       <c r="E103" s="6"/>
@@ -2697,7 +2706,7 @@
     <row r="104" spans="1:5">
       <c r="A104" s="7"/>
       <c r="B104" s="9"/>
-      <c r="C104" s="11" t="s">
+      <c r="C104" s="18" t="s">
         <v>110</v>
       </c>
       <c r="E104" s="6"/>
@@ -2707,7 +2716,7 @@
         <v>111</v>
       </c>
       <c r="B105" s="9"/>
-      <c r="C105" s="11" t="s">
+      <c r="C105" s="18" t="s">
         <v>112</v>
       </c>
       <c r="E105" s="6"/>
@@ -2715,7 +2724,7 @@
     <row r="106" spans="1:5">
       <c r="A106" s="7"/>
       <c r="B106" s="9"/>
-      <c r="C106" s="11" t="s">
+      <c r="C106" s="18" t="s">
         <v>113</v>
       </c>
       <c r="E106" s="6"/>
@@ -2723,7 +2732,7 @@
     <row r="107" spans="1:5">
       <c r="A107" s="7"/>
       <c r="B107" s="9"/>
-      <c r="C107" s="11" t="s">
+      <c r="C107" s="18" t="s">
         <v>114</v>
       </c>
       <c r="E107" s="6"/>
@@ -2731,7 +2740,7 @@
     <row r="108" spans="1:5">
       <c r="A108" s="7"/>
       <c r="B108" s="9"/>
-      <c r="C108" s="11" t="s">
+      <c r="C108" s="18" t="s">
         <v>115</v>
       </c>
       <c r="E108" s="6"/>
@@ -2739,7 +2748,7 @@
     <row r="109" spans="1:5">
       <c r="A109" s="7"/>
       <c r="B109" s="9"/>
-      <c r="C109" s="11" t="s">
+      <c r="C109" s="18" t="s">
         <v>116</v>
       </c>
       <c r="E109" s="6"/>
@@ -2747,17 +2756,17 @@
     <row r="110" ht="27" spans="1:5">
       <c r="A110" s="12"/>
       <c r="B110" s="13"/>
-      <c r="C110" s="14" t="s">
+      <c r="C110" s="19" t="s">
         <v>117</v>
       </c>
       <c r="E110" s="6"/>
     </row>
     <row r="111" spans="1:5">
       <c r="A111" s="3"/>
-      <c r="B111" s="19" t="s">
+      <c r="B111" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="C111" s="17" t="s">
+      <c r="C111" s="20" t="s">
         <v>118</v>
       </c>
       <c r="E111" s="6" t="s">
@@ -2775,7 +2784,7 @@
     <row r="113" spans="1:5">
       <c r="A113" s="7"/>
       <c r="B113" s="9"/>
-      <c r="C113" s="11" t="s">
+      <c r="C113" s="18" t="s">
         <v>120</v>
       </c>
       <c r="E113" s="6"/>
@@ -2783,7 +2792,7 @@
     <row r="114" spans="1:5">
       <c r="A114" s="7"/>
       <c r="B114" s="9"/>
-      <c r="C114" s="11" t="s">
+      <c r="C114" s="18" t="s">
         <v>121</v>
       </c>
       <c r="E114" s="6"/>
@@ -2791,7 +2800,7 @@
     <row r="115" spans="1:5">
       <c r="A115" s="7"/>
       <c r="B115" s="9"/>
-      <c r="C115" s="11" t="s">
+      <c r="C115" s="18" t="s">
         <v>122</v>
       </c>
       <c r="E115" s="6"/>
@@ -2801,7 +2810,7 @@
         <v>123</v>
       </c>
       <c r="B116" s="9"/>
-      <c r="C116" s="11" t="s">
+      <c r="C116" s="18" t="s">
         <v>124</v>
       </c>
       <c r="E116" s="6"/>
@@ -2809,7 +2818,7 @@
     <row r="117" spans="1:5">
       <c r="A117" s="7"/>
       <c r="B117" s="9"/>
-      <c r="C117" s="11" t="s">
+      <c r="C117" s="18" t="s">
         <v>125</v>
       </c>
       <c r="E117" s="6"/>
@@ -2817,7 +2826,7 @@
     <row r="118" spans="1:5">
       <c r="A118" s="7"/>
       <c r="B118" s="9"/>
-      <c r="C118" s="11" t="s">
+      <c r="C118" s="18" t="s">
         <v>126</v>
       </c>
       <c r="E118" s="6"/>
@@ -2825,7 +2834,7 @@
     <row r="119" spans="1:5">
       <c r="A119" s="7"/>
       <c r="B119" s="9"/>
-      <c r="C119" s="11" t="s">
+      <c r="C119" s="18" t="s">
         <v>127</v>
       </c>
       <c r="E119" s="6"/>
@@ -2833,7 +2842,7 @@
     <row r="120" spans="1:5">
       <c r="A120" s="7"/>
       <c r="B120" s="9"/>
-      <c r="C120" s="11" t="s">
+      <c r="C120" s="18" t="s">
         <v>128</v>
       </c>
       <c r="E120" s="6"/>
@@ -2841,7 +2850,7 @@
     <row r="121" spans="1:5">
       <c r="A121" s="7"/>
       <c r="B121" s="9"/>
-      <c r="C121" s="11" t="s">
+      <c r="C121" s="18" t="s">
         <v>129</v>
       </c>
       <c r="E121" s="6"/>
@@ -2849,7 +2858,7 @@
     <row r="122" spans="1:5">
       <c r="A122" s="7"/>
       <c r="B122" s="9"/>
-      <c r="C122" s="11" t="s">
+      <c r="C122" s="18" t="s">
         <v>130</v>
       </c>
       <c r="E122" s="6"/>
@@ -2867,7 +2876,7 @@
     <row r="124" spans="1:5">
       <c r="A124" s="7"/>
       <c r="B124" s="9"/>
-      <c r="C124" s="11" t="s">
+      <c r="C124" s="18" t="s">
         <v>132</v>
       </c>
       <c r="E124" s="6"/>
@@ -2875,7 +2884,7 @@
     <row r="125" spans="1:5">
       <c r="A125" s="7"/>
       <c r="B125" s="9"/>
-      <c r="C125" s="11" t="s">
+      <c r="C125" s="18" t="s">
         <v>133</v>
       </c>
       <c r="E125" s="6"/>
@@ -2883,7 +2892,7 @@
     <row r="126" spans="1:5">
       <c r="A126" s="7"/>
       <c r="B126" s="9"/>
-      <c r="C126" s="11" t="s">
+      <c r="C126" s="18" t="s">
         <v>134</v>
       </c>
       <c r="E126" s="6"/>
@@ -2893,7 +2902,7 @@
         <v>135</v>
       </c>
       <c r="B127" s="9"/>
-      <c r="C127" s="11" t="s">
+      <c r="C127" s="18" t="s">
         <v>136</v>
       </c>
       <c r="E127" s="6"/>
@@ -2901,7 +2910,7 @@
     <row r="128" spans="1:5">
       <c r="A128" s="7"/>
       <c r="B128" s="9"/>
-      <c r="C128" s="11" t="s">
+      <c r="C128" s="18" t="s">
         <v>137</v>
       </c>
       <c r="E128" s="6"/>
@@ -2909,7 +2918,7 @@
     <row r="129" spans="1:5">
       <c r="A129" s="7"/>
       <c r="B129" s="9"/>
-      <c r="C129" s="11" t="s">
+      <c r="C129" s="18" t="s">
         <v>138</v>
       </c>
       <c r="E129" s="6"/>
@@ -2917,7 +2926,7 @@
     <row r="130" spans="1:5">
       <c r="A130" s="7"/>
       <c r="B130" s="9"/>
-      <c r="C130" s="11" t="s">
+      <c r="C130" s="18" t="s">
         <v>139</v>
       </c>
       <c r="E130" s="6"/>
@@ -2925,7 +2934,7 @@
     <row r="131" spans="1:5">
       <c r="A131" s="7"/>
       <c r="B131" s="9"/>
-      <c r="C131" s="11" t="s">
+      <c r="C131" s="18" t="s">
         <v>140</v>
       </c>
       <c r="E131" s="6"/>
@@ -2933,7 +2942,7 @@
     <row r="132" spans="1:5">
       <c r="A132" s="7"/>
       <c r="B132" s="9"/>
-      <c r="C132" s="11" t="s">
+      <c r="C132" s="18" t="s">
         <v>141</v>
       </c>
       <c r="E132" s="6"/>
@@ -2941,7 +2950,7 @@
     <row r="133" ht="27" spans="1:5">
       <c r="A133" s="12"/>
       <c r="B133" s="13"/>
-      <c r="C133" s="14" t="s">
+      <c r="C133" s="19" t="s">
         <v>142</v>
       </c>
       <c r="E133" s="6"/>
@@ -2959,7 +2968,7 @@
       <c r="B135" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="C135" s="11" t="s">
+      <c r="C135" s="18" t="s">
         <v>144</v>
       </c>
       <c r="E135" s="6"/>
@@ -2967,7 +2976,7 @@
     <row r="136" spans="1:5">
       <c r="A136" s="7"/>
       <c r="B136" s="9"/>
-      <c r="C136" s="11" t="s">
+      <c r="C136" s="18" t="s">
         <v>145</v>
       </c>
       <c r="E136" s="6"/>
@@ -2975,7 +2984,7 @@
     <row r="137" spans="1:5">
       <c r="A137" s="7"/>
       <c r="B137" s="9"/>
-      <c r="C137" s="11" t="s">
+      <c r="C137" s="18" t="s">
         <v>146</v>
       </c>
       <c r="E137" s="6"/>
@@ -2983,7 +2992,7 @@
     <row r="138" spans="1:5">
       <c r="A138" s="7"/>
       <c r="B138" s="9"/>
-      <c r="C138" s="11" t="s">
+      <c r="C138" s="18" t="s">
         <v>147</v>
       </c>
       <c r="E138" s="6"/>
@@ -2991,7 +3000,7 @@
     <row r="139" spans="1:5">
       <c r="A139" s="7"/>
       <c r="B139" s="9"/>
-      <c r="C139" s="11" t="s">
+      <c r="C139" s="18" t="s">
         <v>148</v>
       </c>
       <c r="E139" s="6"/>
@@ -2999,7 +3008,7 @@
     <row r="140" spans="1:5">
       <c r="A140" s="7"/>
       <c r="B140" s="9"/>
-      <c r="C140" s="11" t="s">
+      <c r="C140" s="18" t="s">
         <v>149</v>
       </c>
       <c r="E140" s="6"/>
@@ -3007,7 +3016,7 @@
     <row r="141" spans="1:5">
       <c r="A141" s="7"/>
       <c r="B141" s="9"/>
-      <c r="C141" s="11" t="s">
+      <c r="C141" s="18" t="s">
         <v>150</v>
       </c>
       <c r="E141" s="6"/>
@@ -3017,7 +3026,7 @@
         <v>151</v>
       </c>
       <c r="B142" s="9"/>
-      <c r="C142" s="11" t="s">
+      <c r="C142" s="18" t="s">
         <v>152</v>
       </c>
       <c r="E142" s="6"/>
@@ -3025,7 +3034,7 @@
     <row r="143" spans="1:5">
       <c r="A143" s="7"/>
       <c r="B143" s="9"/>
-      <c r="C143" s="11" t="s">
+      <c r="C143" s="18" t="s">
         <v>153</v>
       </c>
       <c r="E143" s="6"/>
@@ -3033,7 +3042,7 @@
     <row r="144" spans="1:5">
       <c r="A144" s="7"/>
       <c r="B144" s="9"/>
-      <c r="C144" s="11" t="s">
+      <c r="C144" s="18" t="s">
         <v>154</v>
       </c>
       <c r="E144" s="6"/>
@@ -3041,7 +3050,7 @@
     <row r="145" spans="1:5">
       <c r="A145" s="7"/>
       <c r="B145" s="9"/>
-      <c r="C145" s="11" t="s">
+      <c r="C145" s="18" t="s">
         <v>155</v>
       </c>
       <c r="E145" s="6"/>
@@ -3049,7 +3058,7 @@
     <row r="146" spans="1:5">
       <c r="A146" s="7"/>
       <c r="B146" s="9"/>
-      <c r="C146" s="11" t="s">
+      <c r="C146" s="18" t="s">
         <v>156</v>
       </c>
       <c r="E146" s="6"/>
@@ -3057,7 +3066,7 @@
     <row r="147" spans="1:5">
       <c r="A147" s="7"/>
       <c r="B147" s="9"/>
-      <c r="C147" s="11" t="s">
+      <c r="C147" s="18" t="s">
         <v>157</v>
       </c>
       <c r="E147" s="6"/>
@@ -3065,7 +3074,7 @@
     <row r="148" spans="1:5">
       <c r="A148" s="7"/>
       <c r="B148" s="9"/>
-      <c r="C148" s="11" t="s">
+      <c r="C148" s="18" t="s">
         <v>158</v>
       </c>
       <c r="E148" s="6"/>
@@ -3073,7 +3082,7 @@
     <row r="149" spans="1:5">
       <c r="A149" s="7"/>
       <c r="B149" s="9"/>
-      <c r="C149" s="11" t="s">
+      <c r="C149" s="18" t="s">
         <v>159</v>
       </c>
       <c r="E149" s="6"/>
@@ -3081,7 +3090,7 @@
     <row r="150" spans="1:5">
       <c r="A150" s="7"/>
       <c r="B150" s="9"/>
-      <c r="C150" s="11" t="s">
+      <c r="C150" s="18" t="s">
         <v>160</v>
       </c>
       <c r="E150" s="6"/>
@@ -3089,7 +3098,7 @@
     <row r="151" spans="1:5">
       <c r="A151" s="7"/>
       <c r="B151" s="9"/>
-      <c r="C151" s="11" t="s">
+      <c r="C151" s="18" t="s">
         <v>161</v>
       </c>
       <c r="E151" s="6"/>
@@ -3097,7 +3106,7 @@
     <row r="152" ht="27" spans="1:5">
       <c r="A152" s="12"/>
       <c r="B152" s="13"/>
-      <c r="C152" s="14" t="s">
+      <c r="C152" s="19" t="s">
         <v>162</v>
       </c>
       <c r="E152" s="6"/>
@@ -3115,7 +3124,7 @@
       <c r="B154" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C154" s="11" t="s">
+      <c r="C154" s="18" t="s">
         <v>164</v>
       </c>
       <c r="E154" s="6"/>
@@ -3123,7 +3132,7 @@
     <row r="155" spans="1:5">
       <c r="A155" s="7"/>
       <c r="B155" s="9"/>
-      <c r="C155" s="11" t="s">
+      <c r="C155" s="18" t="s">
         <v>165</v>
       </c>
       <c r="E155" s="6"/>
@@ -3131,7 +3140,7 @@
     <row r="156" spans="1:5">
       <c r="A156" s="7"/>
       <c r="B156" s="9"/>
-      <c r="C156" s="11" t="s">
+      <c r="C156" s="18" t="s">
         <v>166</v>
       </c>
       <c r="E156" s="6"/>
@@ -3139,7 +3148,7 @@
     <row r="157" spans="1:5">
       <c r="A157" s="7"/>
       <c r="B157" s="9"/>
-      <c r="C157" s="11" t="s">
+      <c r="C157" s="18" t="s">
         <v>167</v>
       </c>
       <c r="E157" s="6"/>
@@ -3147,7 +3156,7 @@
     <row r="158" spans="1:5">
       <c r="A158" s="7"/>
       <c r="B158" s="9"/>
-      <c r="C158" s="11" t="s">
+      <c r="C158" s="18" t="s">
         <v>168</v>
       </c>
       <c r="E158" s="6"/>
@@ -3157,7 +3166,7 @@
         <v>169</v>
       </c>
       <c r="B159" s="9"/>
-      <c r="C159" s="11" t="s">
+      <c r="C159" s="18" t="s">
         <v>170</v>
       </c>
       <c r="E159" s="6"/>
@@ -3165,7 +3174,7 @@
     <row r="160" spans="1:5">
       <c r="A160" s="7"/>
       <c r="B160" s="9"/>
-      <c r="C160" s="11" t="s">
+      <c r="C160" s="18" t="s">
         <v>171</v>
       </c>
       <c r="E160" s="6"/>
@@ -3173,7 +3182,7 @@
     <row r="161" ht="52.5" spans="1:5">
       <c r="A161" s="7"/>
       <c r="B161" s="9"/>
-      <c r="C161" s="20" t="s">
+      <c r="C161" s="23" t="s">
         <v>172</v>
       </c>
       <c r="E161" s="6"/>
@@ -3181,7 +3190,7 @@
     <row r="162" spans="1:5">
       <c r="A162" s="7"/>
       <c r="B162" s="9"/>
-      <c r="C162" s="11" t="s">
+      <c r="C162" s="18" t="s">
         <v>173</v>
       </c>
       <c r="E162" s="6"/>
@@ -3189,7 +3198,7 @@
     <row r="163" spans="1:5">
       <c r="A163" s="7"/>
       <c r="B163" s="9"/>
-      <c r="C163" s="11" t="s">
+      <c r="C163" s="18" t="s">
         <v>174</v>
       </c>
       <c r="E163" s="6"/>
@@ -3197,7 +3206,7 @@
     <row r="164" spans="1:5">
       <c r="A164" s="7"/>
       <c r="B164" s="9"/>
-      <c r="C164" s="11" t="s">
+      <c r="C164" s="18" t="s">
         <v>175</v>
       </c>
       <c r="E164" s="6"/>
@@ -3205,7 +3214,7 @@
     <row r="165" spans="1:5">
       <c r="A165" s="7"/>
       <c r="B165" s="9"/>
-      <c r="C165" s="21" t="s">
+      <c r="C165" s="24" t="s">
         <v>176</v>
       </c>
       <c r="E165" s="6"/>
@@ -3213,7 +3222,7 @@
     <row r="166" spans="1:5">
       <c r="A166" s="7"/>
       <c r="B166" s="9"/>
-      <c r="C166" s="21" t="s">
+      <c r="C166" s="24" t="s">
         <v>177</v>
       </c>
       <c r="E166" s="6"/>
@@ -3221,7 +3230,7 @@
     <row r="167" spans="1:5">
       <c r="A167" s="7"/>
       <c r="B167" s="9"/>
-      <c r="C167" s="21" t="s">
+      <c r="C167" s="24" t="s">
         <v>178</v>
       </c>
       <c r="E167" s="6"/>
@@ -3229,7 +3238,7 @@
     <row r="168" spans="1:5">
       <c r="A168" s="7"/>
       <c r="B168" s="9"/>
-      <c r="C168" s="21" t="s">
+      <c r="C168" s="24" t="s">
         <v>179</v>
       </c>
       <c r="E168" s="6"/>
@@ -3237,7 +3246,7 @@
     <row r="169" spans="1:5">
       <c r="A169" s="7"/>
       <c r="B169" s="9"/>
-      <c r="C169" s="21" t="s">
+      <c r="C169" s="24" t="s">
         <v>180</v>
       </c>
       <c r="E169" s="6"/>
@@ -3245,13 +3254,13 @@
     <row r="170" spans="1:5">
       <c r="A170" s="7"/>
       <c r="B170" s="9"/>
-      <c r="C170" s="21"/>
+      <c r="C170" s="24"/>
       <c r="E170" s="6"/>
     </row>
     <row r="171" spans="1:5">
       <c r="A171" s="7"/>
       <c r="B171" s="9"/>
-      <c r="C171" s="21" t="s">
+      <c r="C171" s="24" t="s">
         <v>181</v>
       </c>
       <c r="E171" s="6"/>
@@ -3259,7 +3268,7 @@
     <row r="172" ht="27" spans="1:5">
       <c r="A172" s="12"/>
       <c r="B172" s="13"/>
-      <c r="C172" s="22" t="s">
+      <c r="C172" s="25" t="s">
         <v>182</v>
       </c>
       <c r="E172" s="6"/>
@@ -3267,10 +3276,10 @@
     <row r="173" spans="1:5">
       <c r="A173" s="3"/>
       <c r="B173" s="4"/>
-      <c r="C173" s="17" t="s">
+      <c r="C173" s="20" t="s">
         <v>183</v>
       </c>
-      <c r="E173" s="23" t="s">
+      <c r="E173" s="26" t="s">
         <v>184</v>
       </c>
     </row>
@@ -3282,57 +3291,57 @@
       <c r="C174" s="10" t="s">
         <v>185</v>
       </c>
-      <c r="E174" s="23"/>
+      <c r="E174" s="26"/>
     </row>
     <row r="175" spans="1:5">
       <c r="A175" s="7"/>
       <c r="B175" s="9"/>
-      <c r="C175" s="11" t="s">
+      <c r="C175" s="18" t="s">
         <v>186</v>
       </c>
-      <c r="E175" s="23"/>
+      <c r="E175" s="26"/>
     </row>
     <row r="176" spans="1:5">
       <c r="A176" s="7"/>
       <c r="B176" s="9"/>
-      <c r="C176" s="11" t="s">
+      <c r="C176" s="18" t="s">
         <v>187</v>
       </c>
-      <c r="E176" s="23"/>
+      <c r="E176" s="26"/>
     </row>
     <row r="177" spans="1:5">
       <c r="A177" s="7"/>
       <c r="B177" s="9"/>
-      <c r="C177" s="11" t="s">
+      <c r="C177" s="18" t="s">
         <v>188</v>
       </c>
-      <c r="E177" s="23"/>
+      <c r="E177" s="26"/>
     </row>
     <row r="178" spans="1:5">
       <c r="A178" s="7"/>
       <c r="B178" s="9"/>
-      <c r="C178" s="11" t="s">
+      <c r="C178" s="18" t="s">
         <v>189</v>
       </c>
-      <c r="E178" s="23"/>
+      <c r="E178" s="26"/>
     </row>
     <row r="179" spans="1:5">
       <c r="A179" s="7" t="s">
         <v>190</v>
       </c>
       <c r="B179" s="9"/>
-      <c r="C179" s="11" t="s">
+      <c r="C179" s="18" t="s">
         <v>191</v>
       </c>
-      <c r="E179" s="23"/>
+      <c r="E179" s="26"/>
     </row>
     <row r="180" spans="1:5">
       <c r="A180" s="7"/>
       <c r="B180" s="9"/>
-      <c r="C180" s="11" t="s">
+      <c r="C180" s="18" t="s">
         <v>192</v>
       </c>
-      <c r="E180" s="23"/>
+      <c r="E180" s="26"/>
     </row>
     <row r="181" spans="1:5">
       <c r="A181" s="7"/>
@@ -3340,166 +3349,166 @@
       <c r="C181" s="10" t="s">
         <v>193</v>
       </c>
-      <c r="E181" s="23"/>
+      <c r="E181" s="26"/>
     </row>
     <row r="182" spans="1:5">
       <c r="A182" s="7"/>
       <c r="B182" s="9"/>
-      <c r="C182" s="11" t="s">
+      <c r="C182" s="18" t="s">
         <v>194</v>
       </c>
-      <c r="E182" s="23"/>
+      <c r="E182" s="26"/>
     </row>
     <row r="183" ht="78.75" spans="1:5">
       <c r="A183" s="7"/>
       <c r="B183" s="9"/>
-      <c r="C183" s="20" t="s">
+      <c r="C183" s="23" t="s">
         <v>195</v>
       </c>
-      <c r="E183" s="23"/>
+      <c r="E183" s="26"/>
     </row>
     <row r="184" spans="1:5">
       <c r="A184" s="7"/>
       <c r="B184" s="9"/>
-      <c r="C184" s="11" t="s">
+      <c r="C184" s="18" t="s">
         <v>196</v>
       </c>
-      <c r="E184" s="23"/>
+      <c r="E184" s="26"/>
     </row>
     <row r="185" spans="1:5">
       <c r="A185" s="7"/>
       <c r="B185" s="9"/>
-      <c r="C185" s="11" t="s">
+      <c r="C185" s="18" t="s">
         <v>197</v>
       </c>
-      <c r="E185" s="23"/>
+      <c r="E185" s="26"/>
     </row>
     <row r="186" spans="1:5">
       <c r="A186" s="7"/>
       <c r="B186" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C186" s="24" t="s">
+      <c r="C186" s="27" t="s">
         <v>198</v>
       </c>
-      <c r="E186" s="23"/>
+      <c r="E186" s="26"/>
     </row>
     <row r="187" spans="1:5">
       <c r="A187" s="7"/>
       <c r="B187" s="9"/>
-      <c r="C187" s="25" t="s">
+      <c r="C187" s="28" t="s">
         <v>199</v>
       </c>
-      <c r="E187" s="23"/>
+      <c r="E187" s="26"/>
     </row>
     <row r="188" spans="1:5">
       <c r="A188" s="7"/>
       <c r="B188" s="9"/>
-      <c r="C188" s="25" t="s">
+      <c r="C188" s="28" t="s">
         <v>200</v>
       </c>
-      <c r="E188" s="23"/>
+      <c r="E188" s="26"/>
     </row>
     <row r="189" spans="1:5">
       <c r="A189" s="7"/>
       <c r="B189" s="9"/>
-      <c r="C189" s="26" t="s">
+      <c r="C189" s="29" t="s">
         <v>201</v>
       </c>
-      <c r="E189" s="23"/>
+      <c r="E189" s="26"/>
     </row>
     <row r="190" ht="51" spans="1:5">
       <c r="A190" s="7" t="s">
         <v>202</v>
       </c>
       <c r="B190" s="9"/>
-      <c r="C190" s="26" t="s">
+      <c r="C190" s="29" t="s">
         <v>203</v>
       </c>
-      <c r="E190" s="23"/>
+      <c r="E190" s="26"/>
     </row>
     <row r="191" spans="1:5">
       <c r="A191" s="7"/>
       <c r="B191" s="9"/>
-      <c r="C191" s="26" t="s">
+      <c r="C191" s="29" t="s">
         <v>204</v>
       </c>
-      <c r="E191" s="23"/>
+      <c r="E191" s="26"/>
     </row>
     <row r="192" spans="1:5">
       <c r="A192" s="7"/>
       <c r="B192" s="9"/>
-      <c r="C192" s="26" t="s">
+      <c r="C192" s="29" t="s">
         <v>205</v>
       </c>
-      <c r="E192" s="23"/>
+      <c r="E192" s="26"/>
     </row>
     <row r="193" spans="1:5">
       <c r="A193" s="7"/>
       <c r="B193" s="9"/>
-      <c r="C193" s="26" t="s">
+      <c r="C193" s="29" t="s">
         <v>206</v>
       </c>
-      <c r="E193" s="23"/>
+      <c r="E193" s="26"/>
     </row>
     <row r="194" spans="1:5">
       <c r="A194" s="7"/>
       <c r="B194" s="9"/>
-      <c r="C194" s="26" t="s">
+      <c r="C194" s="29" t="s">
         <v>207</v>
       </c>
-      <c r="E194" s="23"/>
+      <c r="E194" s="26"/>
     </row>
     <row r="195" spans="1:5">
       <c r="A195" s="7"/>
       <c r="B195" s="9"/>
-      <c r="C195" s="26" t="s">
+      <c r="C195" s="29" t="s">
         <v>208</v>
       </c>
-      <c r="E195" s="23"/>
+      <c r="E195" s="26"/>
     </row>
     <row r="196" spans="1:5">
       <c r="A196" s="7"/>
       <c r="B196" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C196" s="24" t="s">
+      <c r="C196" s="27" t="s">
         <v>209</v>
       </c>
-      <c r="E196" s="23"/>
+      <c r="E196" s="26"/>
     </row>
     <row r="197" spans="1:5">
       <c r="A197" s="7"/>
       <c r="B197" s="9"/>
-      <c r="C197" s="27" t="s">
+      <c r="C197" s="30" t="s">
         <v>210</v>
       </c>
-      <c r="E197" s="23"/>
+      <c r="E197" s="26"/>
     </row>
     <row r="198" spans="1:5">
       <c r="A198" s="7"/>
       <c r="B198" s="9"/>
-      <c r="C198" s="24" t="s">
+      <c r="C198" s="27" t="s">
         <v>211</v>
       </c>
-      <c r="E198" s="23"/>
+      <c r="E198" s="26"/>
     </row>
     <row r="199" spans="1:5">
       <c r="A199" s="7" t="s">
         <v>212</v>
       </c>
       <c r="B199" s="9"/>
-      <c r="C199" s="27" t="s">
+      <c r="C199" s="30" t="s">
         <v>213</v>
       </c>
-      <c r="E199" s="23"/>
+      <c r="E199" s="26"/>
     </row>
     <row r="200" spans="2:5">
       <c r="B200" s="9"/>
-      <c r="C200" s="27" t="s">
+      <c r="C200" s="30" t="s">
         <v>214</v>
       </c>
-      <c r="E200" s="23"/>
+      <c r="E200" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="21">

</xml_diff>

<commit_message>
updated setup for maven
</commit_message>
<xml_diff>
--- a/TOC/Course_Content_Angular14_Training.xlsx
+++ b/TOC/Course_Content_Angular14_Training.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26529"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Online Training\Coforge-Angular14-July-2023\TOC\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34A2A833-8171-4FF7-9945-B2F889019870}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="19635" windowHeight="7620"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -664,14 +670,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="25">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -713,152 +713,8 @@
       <name val="Arial"/>
       <charset val="134"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="36">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -867,19 +723,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.39994506668294322"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.39994506668294322"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -907,170 +763,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="22">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -1229,282 +923,28 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1530,62 +970,34 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Currency" xfId="2" builtinId="4"/>
-    <cellStyle name="Percent" xfId="3" builtinId="5"/>
-    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
-    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
-    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
-    <cellStyle name="Note" xfId="8" builtinId="10"/>
-    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
-    <cellStyle name="Title" xfId="10" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
-    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
-    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
-    <cellStyle name="Input" xfId="16" builtinId="20"/>
-    <cellStyle name="Output" xfId="17" builtinId="21"/>
-    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
-    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
-    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
-    <cellStyle name="Total" xfId="21" builtinId="25"/>
-    <cellStyle name="Good" xfId="22" builtinId="26"/>
-    <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
-    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
-    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
-    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
-    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
-    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
-    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
-    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
-    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
-    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
-    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
-    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
-    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1843,29 +1255,29 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E200"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" topLeftCell="A89" workbookViewId="0">
-      <selection activeCell="C200" sqref="C200"/>
+    <sheetView tabSelected="1" topLeftCell="A163" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C174" sqref="C174:C182"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="26.25" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="25.8"/>
   <cols>
-    <col min="1" max="1" width="16.1142857142857" style="1" customWidth="1"/>
-    <col min="2" max="2" width="24.1809523809524" style="1" customWidth="1"/>
-    <col min="3" max="3" width="95.2666666666667" style="1" customWidth="1"/>
+    <col min="1" max="1" width="16.109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24.21875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="95.21875" style="1" customWidth="1"/>
     <col min="4" max="4" width="9" style="1"/>
-    <col min="5" max="5" width="25.0952380952381" style="1" customWidth="1"/>
+    <col min="5" max="5" width="25.109375" style="1" customWidth="1"/>
     <col min="6" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3">
+    <row r="1" spans="1:5">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1877,1678 +1289,1677 @@
       <c r="C3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="33" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="7"/>
-      <c r="C4" s="8" t="s">
+      <c r="A4" s="6"/>
+      <c r="C4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="6"/>
+      <c r="E4" s="33"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="7"/>
-      <c r="B5" s="9" t="s">
+      <c r="A5" s="6"/>
+      <c r="B5" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="6"/>
+      <c r="E5" s="33"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="7"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="11" t="s">
+      <c r="A6" s="6"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="6"/>
+      <c r="E6" s="33"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="7"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="11" t="s">
+      <c r="A7" s="6"/>
+      <c r="B7" s="30"/>
+      <c r="C7" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="6"/>
+      <c r="E7" s="33"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="9"/>
-      <c r="C8" s="11" t="s">
+      <c r="B8" s="30"/>
+      <c r="C8" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="6"/>
+      <c r="E8" s="33"/>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="7"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="11" t="s">
+      <c r="A9" s="6"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="6"/>
+      <c r="E9" s="33"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="7"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="11" t="s">
+      <c r="A10" s="6"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="6"/>
+      <c r="E10" s="33"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="7"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="11" t="s">
+      <c r="A11" s="6"/>
+      <c r="B11" s="30"/>
+      <c r="C11" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="6"/>
+      <c r="E11" s="33"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="7"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="11" t="s">
+      <c r="A12" s="6"/>
+      <c r="B12" s="30"/>
+      <c r="C12" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E12" s="6"/>
+      <c r="E12" s="33"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="7"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="11" t="s">
+      <c r="A13" s="6"/>
+      <c r="B13" s="30"/>
+      <c r="C13" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="E13" s="6"/>
+      <c r="E13" s="33"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="7"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="11" t="s">
+      <c r="A14" s="6"/>
+      <c r="B14" s="30"/>
+      <c r="C14" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E14" s="6"/>
-    </row>
-    <row r="15" ht="27" spans="1:5">
-      <c r="A15" s="12"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="14" t="s">
+      <c r="E14" s="33"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="10"/>
+      <c r="B15" s="31"/>
+      <c r="C15" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="E15" s="6"/>
+      <c r="E15" s="33"/>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="3"/>
       <c r="B16" s="4"/>
-      <c r="C16" s="15" t="s">
+      <c r="C16" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="E16" s="33" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="7"/>
-      <c r="B17" s="9" t="s">
+      <c r="A17" s="6"/>
+      <c r="B17" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="E17" s="6"/>
+      <c r="E17" s="33"/>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="7"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="11" t="s">
+      <c r="A18" s="6"/>
+      <c r="B18" s="30"/>
+      <c r="C18" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E18" s="6"/>
+      <c r="E18" s="33"/>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="7"/>
-      <c r="B19" s="9"/>
-      <c r="C19" s="11" t="s">
+      <c r="A19" s="6"/>
+      <c r="B19" s="30"/>
+      <c r="C19" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E19" s="6"/>
+      <c r="E19" s="33"/>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="7"/>
-      <c r="B20" s="9"/>
-      <c r="C20" s="11" t="s">
+      <c r="A20" s="6"/>
+      <c r="B20" s="30"/>
+      <c r="C20" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="E20" s="6"/>
+      <c r="E20" s="33"/>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="7"/>
-      <c r="B21" s="9"/>
-      <c r="C21" s="11" t="s">
+      <c r="A21" s="6"/>
+      <c r="B21" s="30"/>
+      <c r="C21" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E21" s="6"/>
+      <c r="E21" s="33"/>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="9"/>
-      <c r="C22" s="11" t="s">
+      <c r="B22" s="30"/>
+      <c r="C22" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="E22" s="6"/>
+      <c r="E22" s="33"/>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="7"/>
-      <c r="B23" s="9"/>
-      <c r="C23" s="11" t="s">
+      <c r="A23" s="6"/>
+      <c r="B23" s="30"/>
+      <c r="C23" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="E23" s="6"/>
+      <c r="E23" s="33"/>
     </row>
     <row r="24" spans="1:5">
-      <c r="A24" s="7"/>
-      <c r="B24" s="9"/>
-      <c r="C24" s="11" t="s">
+      <c r="A24" s="6"/>
+      <c r="B24" s="30"/>
+      <c r="C24" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E24" s="6"/>
+      <c r="E24" s="33"/>
     </row>
     <row r="25" spans="1:5">
-      <c r="A25" s="7"/>
-      <c r="B25" s="9"/>
-      <c r="C25" s="11" t="s">
+      <c r="A25" s="6"/>
+      <c r="B25" s="30"/>
+      <c r="C25" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E25" s="6"/>
+      <c r="E25" s="33"/>
     </row>
     <row r="26" spans="1:5">
-      <c r="A26" s="7"/>
-      <c r="B26" s="9"/>
-      <c r="C26" s="11" t="s">
+      <c r="A26" s="6"/>
+      <c r="B26" s="30"/>
+      <c r="C26" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="E26" s="6"/>
+      <c r="E26" s="33"/>
     </row>
     <row r="27" spans="1:5">
-      <c r="A27" s="7"/>
-      <c r="B27" s="9"/>
-      <c r="C27" s="11" t="s">
+      <c r="A27" s="6"/>
+      <c r="B27" s="30"/>
+      <c r="C27" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="E27" s="6"/>
+      <c r="E27" s="33"/>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="7"/>
-      <c r="B28" s="9"/>
-      <c r="C28" s="11" t="s">
+      <c r="A28" s="6"/>
+      <c r="B28" s="30"/>
+      <c r="C28" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="E28" s="6"/>
+      <c r="E28" s="33"/>
     </row>
     <row r="29" spans="1:5">
-      <c r="A29" s="7"/>
-      <c r="B29" s="9"/>
-      <c r="C29" s="11" t="s">
+      <c r="A29" s="6"/>
+      <c r="B29" s="30"/>
+      <c r="C29" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="E29" s="6"/>
+      <c r="E29" s="33"/>
     </row>
     <row r="30" spans="1:5">
-      <c r="A30" s="7"/>
-      <c r="B30" s="9"/>
-      <c r="C30" s="11" t="s">
+      <c r="A30" s="6"/>
+      <c r="B30" s="30"/>
+      <c r="C30" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E30" s="6"/>
+      <c r="E30" s="33"/>
     </row>
     <row r="31" spans="1:5">
-      <c r="A31" s="7"/>
-      <c r="B31" s="9"/>
-      <c r="C31" s="11" t="s">
+      <c r="A31" s="6"/>
+      <c r="B31" s="30"/>
+      <c r="C31" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="E31" s="6"/>
+      <c r="E31" s="33"/>
     </row>
     <row r="32" spans="1:5">
-      <c r="A32" s="7"/>
-      <c r="B32" s="9"/>
-      <c r="C32" s="11" t="s">
+      <c r="A32" s="6"/>
+      <c r="B32" s="30"/>
+      <c r="C32" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="E32" s="6"/>
+      <c r="E32" s="33"/>
     </row>
     <row r="33" spans="1:5">
-      <c r="A33" s="7"/>
-      <c r="B33" s="9"/>
-      <c r="C33" s="11" t="s">
+      <c r="A33" s="6"/>
+      <c r="B33" s="30"/>
+      <c r="C33" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="E33" s="6"/>
+      <c r="E33" s="33"/>
     </row>
     <row r="34" spans="1:5">
-      <c r="A34" s="7"/>
-      <c r="B34" s="9"/>
-      <c r="C34" s="11" t="s">
+      <c r="A34" s="6"/>
+      <c r="B34" s="30"/>
+      <c r="C34" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="E34" s="6"/>
+      <c r="E34" s="33"/>
     </row>
     <row r="35" spans="1:5">
-      <c r="A35" s="7"/>
-      <c r="B35" s="9"/>
-      <c r="C35" s="11" t="s">
+      <c r="A35" s="6"/>
+      <c r="B35" s="30"/>
+      <c r="C35" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E35" s="6"/>
+      <c r="E35" s="33"/>
     </row>
     <row r="36" spans="1:5">
-      <c r="A36" s="7"/>
-      <c r="B36" s="9"/>
-      <c r="C36" s="11" t="s">
+      <c r="A36" s="6"/>
+      <c r="B36" s="30"/>
+      <c r="C36" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E36" s="6"/>
-    </row>
-    <row r="37" ht="27" spans="1:5">
-      <c r="A37" s="12"/>
-      <c r="B37" s="13"/>
-      <c r="C37" s="14" t="s">
+      <c r="E36" s="33"/>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="10"/>
+      <c r="B37" s="31"/>
+      <c r="C37" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="E37" s="6"/>
+      <c r="E37" s="33"/>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="3"/>
       <c r="B38" s="4"/>
-      <c r="C38" s="16" t="s">
+      <c r="C38" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="E38" s="6" t="s">
+      <c r="E38" s="33" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:5">
-      <c r="A39" s="7"/>
-      <c r="B39" s="9" t="s">
+      <c r="A39" s="6"/>
+      <c r="B39" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="C39" s="11" t="s">
+      <c r="C39" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="E39" s="6"/>
+      <c r="E39" s="33"/>
     </row>
     <row r="40" spans="1:5">
-      <c r="A40" s="7" t="s">
+      <c r="A40" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B40" s="9"/>
-      <c r="C40" s="11" t="s">
+      <c r="B40" s="30"/>
+      <c r="C40" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="E40" s="6"/>
+      <c r="E40" s="33"/>
     </row>
     <row r="41" spans="1:5">
-      <c r="A41" s="7"/>
-      <c r="B41" s="9"/>
-      <c r="C41" s="11" t="s">
+      <c r="A41" s="6"/>
+      <c r="B41" s="30"/>
+      <c r="C41" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="E41" s="6"/>
+      <c r="E41" s="33"/>
     </row>
     <row r="42" spans="1:5">
-      <c r="A42" s="7"/>
-      <c r="B42" s="9"/>
-      <c r="C42" s="11" t="s">
+      <c r="A42" s="6"/>
+      <c r="B42" s="30"/>
+      <c r="C42" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E42" s="6"/>
-    </row>
-    <row r="43" ht="27" spans="1:5">
-      <c r="A43" s="12"/>
-      <c r="B43" s="13"/>
-      <c r="C43" s="14" t="s">
+      <c r="E42" s="33"/>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="10"/>
+      <c r="B43" s="31"/>
+      <c r="C43" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="E43" s="6"/>
+      <c r="E43" s="33"/>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="3"/>
       <c r="B44" s="4"/>
-      <c r="C44" s="16" t="s">
+      <c r="C44" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="E44" s="6"/>
+      <c r="E44" s="33"/>
     </row>
     <row r="45" spans="1:5">
-      <c r="A45" s="7"/>
-      <c r="B45" s="9" t="s">
+      <c r="A45" s="6"/>
+      <c r="B45" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="C45" s="17" t="s">
+      <c r="C45" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="E45" s="6"/>
+      <c r="E45" s="33"/>
     </row>
     <row r="46" spans="1:5">
-      <c r="A46" s="7"/>
-      <c r="B46" s="9"/>
-      <c r="C46" s="17" t="s">
+      <c r="A46" s="6"/>
+      <c r="B46" s="30"/>
+      <c r="C46" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="E46" s="6"/>
+      <c r="E46" s="33"/>
     </row>
     <row r="47" spans="1:5">
-      <c r="A47" s="7"/>
-      <c r="B47" s="9"/>
-      <c r="C47" s="17" t="s">
+      <c r="A47" s="6"/>
+      <c r="B47" s="30"/>
+      <c r="C47" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="E47" s="6"/>
+      <c r="E47" s="33"/>
     </row>
     <row r="48" spans="1:5">
-      <c r="A48" s="7"/>
-      <c r="B48" s="9"/>
-      <c r="C48" s="17" t="s">
+      <c r="A48" s="6"/>
+      <c r="B48" s="30"/>
+      <c r="C48" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="E48" s="6"/>
+      <c r="E48" s="33"/>
     </row>
     <row r="49" spans="1:5">
-      <c r="A49" s="7" t="s">
+      <c r="A49" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B49" s="9"/>
-      <c r="C49" s="17" t="s">
+      <c r="B49" s="30"/>
+      <c r="C49" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="E49" s="6"/>
+      <c r="E49" s="33"/>
     </row>
     <row r="50" spans="1:5">
-      <c r="A50" s="7"/>
-      <c r="B50" s="9"/>
-      <c r="C50" s="17" t="s">
+      <c r="A50" s="6"/>
+      <c r="B50" s="30"/>
+      <c r="C50" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="E50" s="6"/>
+      <c r="E50" s="33"/>
     </row>
     <row r="51" spans="1:5">
-      <c r="A51" s="7"/>
-      <c r="B51" s="9"/>
-      <c r="C51" s="17" t="s">
+      <c r="A51" s="6"/>
+      <c r="B51" s="30"/>
+      <c r="C51" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="E51" s="6"/>
+      <c r="E51" s="33"/>
     </row>
     <row r="52" spans="1:5">
-      <c r="A52" s="7"/>
-      <c r="B52" s="9"/>
-      <c r="C52" s="17" t="s">
+      <c r="A52" s="6"/>
+      <c r="B52" s="30"/>
+      <c r="C52" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="E52" s="6"/>
+      <c r="E52" s="33"/>
     </row>
     <row r="53" spans="1:5">
-      <c r="A53" s="7"/>
-      <c r="B53" s="9"/>
-      <c r="C53" s="17" t="s">
+      <c r="A53" s="6"/>
+      <c r="B53" s="30"/>
+      <c r="C53" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="E53" s="6"/>
+      <c r="E53" s="33"/>
     </row>
     <row r="54" spans="1:5">
-      <c r="A54" s="7"/>
-      <c r="B54" s="9"/>
-      <c r="C54" s="17" t="s">
+      <c r="A54" s="6"/>
+      <c r="B54" s="30"/>
+      <c r="C54" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="E54" s="6"/>
+      <c r="E54" s="33"/>
     </row>
     <row r="55" spans="1:5">
-      <c r="A55" s="7"/>
-      <c r="B55" s="9"/>
-      <c r="C55" s="17" t="s">
+      <c r="A55" s="6"/>
+      <c r="B55" s="30"/>
+      <c r="C55" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="E55" s="6"/>
+      <c r="E55" s="33"/>
     </row>
     <row r="56" spans="1:5">
-      <c r="A56" s="7"/>
-      <c r="B56" s="9"/>
-      <c r="C56" s="17" t="s">
+      <c r="A56" s="6"/>
+      <c r="B56" s="30"/>
+      <c r="C56" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="E56" s="6"/>
-    </row>
-    <row r="57" ht="27" spans="1:5">
-      <c r="A57" s="12"/>
-      <c r="B57" s="13"/>
-      <c r="C57" s="17" t="s">
+      <c r="E56" s="33"/>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" s="10"/>
+      <c r="B57" s="31"/>
+      <c r="C57" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="E57" s="6"/>
+      <c r="E57" s="33"/>
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="3"/>
       <c r="B58" s="4"/>
-      <c r="C58" s="18" t="s">
+      <c r="C58" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="E58" s="6" t="s">
+      <c r="E58" s="33" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="59" spans="1:5">
-      <c r="A59" s="7"/>
-      <c r="B59" s="9" t="s">
+      <c r="A59" s="6"/>
+      <c r="B59" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="C59" s="19" t="s">
+      <c r="C59" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="E59" s="6"/>
+      <c r="E59" s="33"/>
     </row>
     <row r="60" spans="1:5">
-      <c r="A60" s="7"/>
-      <c r="B60" s="9"/>
-      <c r="C60" s="17" t="s">
+      <c r="A60" s="6"/>
+      <c r="B60" s="30"/>
+      <c r="C60" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="E60" s="6"/>
+      <c r="E60" s="33"/>
     </row>
     <row r="61" spans="1:5">
-      <c r="A61" s="7"/>
-      <c r="B61" s="9"/>
-      <c r="C61" s="17" t="s">
+      <c r="A61" s="6"/>
+      <c r="B61" s="30"/>
+      <c r="C61" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="E61" s="6"/>
+      <c r="E61" s="33"/>
     </row>
     <row r="62" spans="1:5">
-      <c r="A62" s="7"/>
-      <c r="B62" s="9"/>
-      <c r="C62" s="17" t="s">
+      <c r="A62" s="6"/>
+      <c r="B62" s="30"/>
+      <c r="C62" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="E62" s="6"/>
+      <c r="E62" s="33"/>
     </row>
     <row r="63" spans="1:5">
-      <c r="A63" s="7" t="s">
+      <c r="A63" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="B63" s="9"/>
-      <c r="C63" s="17" t="s">
+      <c r="B63" s="30"/>
+      <c r="C63" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="E63" s="6"/>
+      <c r="E63" s="33"/>
     </row>
     <row r="64" spans="1:5">
-      <c r="A64" s="7"/>
-      <c r="B64" s="9"/>
-      <c r="C64" s="17" t="s">
+      <c r="A64" s="6"/>
+      <c r="B64" s="30"/>
+      <c r="C64" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="E64" s="6"/>
+      <c r="E64" s="33"/>
     </row>
     <row r="65" spans="1:5">
-      <c r="A65" s="7"/>
-      <c r="B65" s="9"/>
-      <c r="C65" s="17" t="s">
+      <c r="A65" s="6"/>
+      <c r="B65" s="30"/>
+      <c r="C65" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="E65" s="6"/>
+      <c r="E65" s="33"/>
     </row>
     <row r="66" spans="1:5">
-      <c r="A66" s="7"/>
-      <c r="B66" s="9"/>
-      <c r="C66" s="17" t="s">
+      <c r="A66" s="6"/>
+      <c r="B66" s="30"/>
+      <c r="C66" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="E66" s="6"/>
+      <c r="E66" s="33"/>
     </row>
     <row r="67" spans="1:5">
-      <c r="A67" s="7"/>
-      <c r="B67" s="9"/>
-      <c r="C67" s="17" t="s">
+      <c r="A67" s="6"/>
+      <c r="B67" s="30"/>
+      <c r="C67" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="E67" s="6"/>
+      <c r="E67" s="33"/>
     </row>
     <row r="68" spans="1:5">
-      <c r="A68" s="7"/>
-      <c r="B68" s="9"/>
-      <c r="C68" s="17" t="s">
+      <c r="A68" s="6"/>
+      <c r="B68" s="30"/>
+      <c r="C68" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="E68" s="6"/>
+      <c r="E68" s="33"/>
     </row>
     <row r="69" spans="1:5">
-      <c r="A69" s="7"/>
-      <c r="B69" s="9"/>
-      <c r="C69" s="17" t="s">
+      <c r="A69" s="6"/>
+      <c r="B69" s="30"/>
+      <c r="C69" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="E69" s="6"/>
+      <c r="E69" s="33"/>
     </row>
     <row r="70" spans="1:5">
-      <c r="A70" s="7"/>
-      <c r="B70" s="9"/>
-      <c r="C70" s="17" t="s">
+      <c r="A70" s="6"/>
+      <c r="B70" s="30"/>
+      <c r="C70" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="E70" s="6"/>
+      <c r="E70" s="33"/>
     </row>
     <row r="71" spans="1:5">
-      <c r="A71" s="7"/>
-      <c r="B71" s="9"/>
-      <c r="C71" s="17" t="s">
+      <c r="A71" s="6"/>
+      <c r="B71" s="30"/>
+      <c r="C71" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="E71" s="6"/>
+      <c r="E71" s="33"/>
     </row>
     <row r="72" spans="1:5">
-      <c r="A72" s="7"/>
-      <c r="B72" s="9"/>
-      <c r="C72" s="17" t="s">
+      <c r="A72" s="6"/>
+      <c r="B72" s="30"/>
+      <c r="C72" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="E72" s="6"/>
+      <c r="E72" s="33"/>
     </row>
     <row r="73" spans="1:5">
-      <c r="A73" s="7"/>
-      <c r="B73" s="9"/>
-      <c r="C73" s="17" t="s">
+      <c r="A73" s="6"/>
+      <c r="B73" s="30"/>
+      <c r="C73" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="E73" s="6"/>
+      <c r="E73" s="33"/>
     </row>
     <row r="74" spans="1:5">
-      <c r="A74" s="7"/>
-      <c r="B74" s="9"/>
-      <c r="C74" s="10" t="s">
+      <c r="A74" s="6"/>
+      <c r="B74" s="30"/>
+      <c r="C74" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="E74" s="6"/>
+      <c r="E74" s="33"/>
     </row>
     <row r="75" spans="1:5">
-      <c r="A75" s="7"/>
-      <c r="B75" s="9"/>
-      <c r="C75" s="17" t="s">
+      <c r="A75" s="6"/>
+      <c r="B75" s="30"/>
+      <c r="C75" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="E75" s="6"/>
+      <c r="E75" s="33"/>
     </row>
     <row r="76" spans="1:5">
-      <c r="A76" s="7"/>
-      <c r="B76" s="9"/>
-      <c r="C76" s="17" t="s">
+      <c r="A76" s="6"/>
+      <c r="B76" s="30"/>
+      <c r="C76" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="E76" s="6"/>
+      <c r="E76" s="33"/>
     </row>
     <row r="77" spans="1:5">
-      <c r="A77" s="7"/>
-      <c r="B77" s="9"/>
-      <c r="C77" s="17" t="s">
+      <c r="A77" s="6"/>
+      <c r="B77" s="30"/>
+      <c r="C77" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="E77" s="6"/>
+      <c r="E77" s="33"/>
     </row>
     <row r="78" spans="1:5">
-      <c r="A78" s="7"/>
-      <c r="B78" s="9"/>
-      <c r="C78" s="17" t="s">
+      <c r="A78" s="6"/>
+      <c r="B78" s="30"/>
+      <c r="C78" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="E78" s="6"/>
-    </row>
-    <row r="79" ht="27" spans="1:5">
-      <c r="A79" s="12"/>
-      <c r="B79" s="13"/>
-      <c r="C79" s="17" t="s">
+      <c r="E78" s="33"/>
+    </row>
+    <row r="79" spans="1:5">
+      <c r="A79" s="10"/>
+      <c r="B79" s="31"/>
+      <c r="C79" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="E79" s="6"/>
+      <c r="E79" s="33"/>
     </row>
     <row r="80" spans="1:5">
       <c r="A80" s="3"/>
-      <c r="B80" s="20" t="s">
+      <c r="B80" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="C80" s="15" t="s">
+      <c r="C80" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="E80" s="6"/>
+      <c r="E80" s="33"/>
     </row>
     <row r="81" spans="1:5">
-      <c r="A81" s="7"/>
-      <c r="B81" s="9"/>
-      <c r="C81" s="17" t="s">
+      <c r="A81" s="6"/>
+      <c r="B81" s="30"/>
+      <c r="C81" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="E81" s="6"/>
+      <c r="E81" s="33"/>
     </row>
     <row r="82" spans="1:5">
-      <c r="A82" s="7"/>
-      <c r="B82" s="9"/>
-      <c r="C82" s="17" t="s">
+      <c r="A82" s="6"/>
+      <c r="B82" s="30"/>
+      <c r="C82" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="E82" s="6"/>
+      <c r="E82" s="33"/>
     </row>
     <row r="83" spans="1:5">
-      <c r="A83" s="7"/>
-      <c r="B83" s="9"/>
-      <c r="C83" s="17" t="s">
+      <c r="A83" s="6"/>
+      <c r="B83" s="30"/>
+      <c r="C83" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="E83" s="6"/>
+      <c r="E83" s="33"/>
     </row>
     <row r="84" spans="1:5">
-      <c r="A84" s="7"/>
-      <c r="B84" s="9"/>
-      <c r="C84" s="17" t="s">
+      <c r="A84" s="6"/>
+      <c r="B84" s="30"/>
+      <c r="C84" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="E84" s="6"/>
+      <c r="E84" s="33"/>
     </row>
     <row r="85" spans="1:5">
-      <c r="A85" s="7"/>
-      <c r="B85" s="9"/>
-      <c r="C85" s="17" t="s">
+      <c r="A85" s="6"/>
+      <c r="B85" s="30"/>
+      <c r="C85" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="E85" s="6"/>
+      <c r="E85" s="33"/>
     </row>
     <row r="86" spans="1:5">
-      <c r="A86" s="7"/>
-      <c r="B86" s="9"/>
-      <c r="C86" s="21" t="s">
+      <c r="A86" s="6"/>
+      <c r="B86" s="30"/>
+      <c r="C86" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="E86" s="6"/>
+      <c r="E86" s="33"/>
     </row>
     <row r="87" spans="1:5">
-      <c r="A87" s="7"/>
-      <c r="B87" s="9"/>
-      <c r="C87" s="21" t="s">
+      <c r="A87" s="6"/>
+      <c r="B87" s="30"/>
+      <c r="C87" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="E87" s="6"/>
+      <c r="E87" s="33"/>
     </row>
     <row r="88" spans="1:5">
-      <c r="A88" s="7" t="s">
+      <c r="A88" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="B88" s="9"/>
-      <c r="C88" s="21" t="s">
+      <c r="B88" s="30"/>
+      <c r="C88" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="E88" s="6"/>
+      <c r="E88" s="33"/>
     </row>
     <row r="89" spans="1:5">
-      <c r="A89" s="7"/>
-      <c r="B89" s="9"/>
-      <c r="C89" s="21" t="s">
+      <c r="A89" s="6"/>
+      <c r="B89" s="30"/>
+      <c r="C89" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="E89" s="6"/>
-    </row>
-    <row r="90" ht="52.5" spans="1:5">
-      <c r="A90" s="7"/>
-      <c r="B90" s="9"/>
-      <c r="C90" s="22" t="s">
+      <c r="E89" s="33"/>
+    </row>
+    <row r="90" spans="1:5" ht="51.6">
+      <c r="A90" s="6"/>
+      <c r="B90" s="30"/>
+      <c r="C90" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="E90" s="6"/>
+      <c r="E90" s="33"/>
     </row>
     <row r="91" spans="1:5">
-      <c r="A91" s="7"/>
-      <c r="B91" s="9"/>
-      <c r="C91" s="21" t="s">
+      <c r="A91" s="6"/>
+      <c r="B91" s="30"/>
+      <c r="C91" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="E91" s="6"/>
+      <c r="E91" s="33"/>
     </row>
     <row r="92" spans="1:5">
-      <c r="A92" s="7"/>
-      <c r="B92" s="9"/>
-      <c r="C92" s="21" t="s">
+      <c r="A92" s="6"/>
+      <c r="B92" s="30"/>
+      <c r="C92" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="E92" s="6"/>
+      <c r="E92" s="33"/>
     </row>
     <row r="93" spans="1:5">
-      <c r="A93" s="7"/>
-      <c r="B93" s="9" t="s">
+      <c r="A93" s="6"/>
+      <c r="B93" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="C93" s="10" t="s">
+      <c r="C93" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="E93" s="6"/>
+      <c r="E93" s="33"/>
     </row>
     <row r="94" spans="1:5">
-      <c r="A94" s="7"/>
-      <c r="B94" s="9"/>
-      <c r="C94" s="21" t="s">
+      <c r="A94" s="6"/>
+      <c r="B94" s="30"/>
+      <c r="C94" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="E94" s="6"/>
+      <c r="E94" s="33"/>
     </row>
     <row r="95" spans="1:5">
-      <c r="A95" s="7"/>
-      <c r="B95" s="9"/>
-      <c r="C95" s="21" t="s">
+      <c r="A95" s="6"/>
+      <c r="B95" s="30"/>
+      <c r="C95" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="E95" s="6"/>
+      <c r="E95" s="33"/>
     </row>
     <row r="96" spans="1:5">
-      <c r="A96" s="7"/>
-      <c r="B96" s="9"/>
-      <c r="C96" s="21" t="s">
+      <c r="A96" s="6"/>
+      <c r="B96" s="30"/>
+      <c r="C96" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="E96" s="6"/>
+      <c r="E96" s="33"/>
     </row>
     <row r="97" spans="1:5">
-      <c r="A97" s="7" t="s">
+      <c r="A97" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="B97" s="9"/>
-      <c r="C97" s="21" t="s">
+      <c r="B97" s="30"/>
+      <c r="C97" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="E97" s="6"/>
+      <c r="E97" s="33"/>
     </row>
     <row r="98" spans="1:5">
-      <c r="A98" s="7"/>
-      <c r="B98" s="9"/>
-      <c r="C98" s="21" t="s">
+      <c r="A98" s="6"/>
+      <c r="B98" s="30"/>
+      <c r="C98" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="E98" s="6"/>
+      <c r="E98" s="33"/>
     </row>
     <row r="99" spans="1:5">
-      <c r="A99" s="7"/>
-      <c r="B99" s="9"/>
-      <c r="C99" s="21" t="s">
+      <c r="A99" s="6"/>
+      <c r="B99" s="30"/>
+      <c r="C99" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="E99" s="6"/>
-    </row>
-    <row r="100" ht="52.5" spans="1:5">
-      <c r="A100" s="7"/>
-      <c r="B100" s="9"/>
-      <c r="C100" s="22" t="s">
+      <c r="E99" s="33"/>
+    </row>
+    <row r="100" spans="1:5" ht="51.6">
+      <c r="A100" s="6"/>
+      <c r="B100" s="30"/>
+      <c r="C100" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="E100" s="6"/>
+      <c r="E100" s="33"/>
     </row>
     <row r="101" spans="1:5">
-      <c r="A101" s="7"/>
-      <c r="B101" s="9"/>
-      <c r="C101" s="17" t="s">
+      <c r="A101" s="6"/>
+      <c r="B101" s="30"/>
+      <c r="C101" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="E101" s="6"/>
+      <c r="E101" s="33"/>
     </row>
     <row r="102" spans="1:5">
-      <c r="A102" s="7"/>
-      <c r="B102" s="9" t="s">
+      <c r="A102" s="6"/>
+      <c r="B102" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="C102" s="10" t="s">
+      <c r="C102" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="E102" s="6"/>
+      <c r="E102" s="33"/>
     </row>
     <row r="103" spans="1:5">
-      <c r="A103" s="7"/>
-      <c r="B103" s="9"/>
-      <c r="C103" s="17" t="s">
+      <c r="A103" s="6"/>
+      <c r="B103" s="30"/>
+      <c r="C103" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="E103" s="6"/>
+      <c r="E103" s="33"/>
     </row>
     <row r="104" spans="1:5">
-      <c r="A104" s="7"/>
-      <c r="B104" s="9"/>
-      <c r="C104" s="17" t="s">
+      <c r="A104" s="6"/>
+      <c r="B104" s="30"/>
+      <c r="C104" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="E104" s="6"/>
+      <c r="E104" s="33"/>
     </row>
     <row r="105" spans="1:5">
-      <c r="A105" s="7" t="s">
+      <c r="A105" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="B105" s="9"/>
-      <c r="C105" s="17" t="s">
+      <c r="B105" s="30"/>
+      <c r="C105" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="E105" s="6"/>
+      <c r="E105" s="33"/>
     </row>
     <row r="106" spans="1:5">
-      <c r="A106" s="7"/>
-      <c r="B106" s="9"/>
-      <c r="C106" s="17" t="s">
+      <c r="A106" s="6"/>
+      <c r="B106" s="30"/>
+      <c r="C106" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="E106" s="6"/>
+      <c r="E106" s="33"/>
     </row>
     <row r="107" spans="1:5">
-      <c r="A107" s="7"/>
-      <c r="B107" s="9"/>
-      <c r="C107" s="17" t="s">
+      <c r="A107" s="6"/>
+      <c r="B107" s="30"/>
+      <c r="C107" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="E107" s="6"/>
+      <c r="E107" s="33"/>
     </row>
     <row r="108" spans="1:5">
-      <c r="A108" s="7"/>
-      <c r="B108" s="9"/>
-      <c r="C108" s="17" t="s">
+      <c r="A108" s="6"/>
+      <c r="B108" s="30"/>
+      <c r="C108" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="E108" s="6"/>
+      <c r="E108" s="33"/>
     </row>
     <row r="109" spans="1:5">
-      <c r="A109" s="7"/>
-      <c r="B109" s="9"/>
-      <c r="C109" s="17" t="s">
+      <c r="A109" s="6"/>
+      <c r="B109" s="30"/>
+      <c r="C109" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="E109" s="6"/>
-    </row>
-    <row r="110" ht="27" spans="1:5">
-      <c r="A110" s="12"/>
-      <c r="B110" s="13"/>
-      <c r="C110" s="17" t="s">
+      <c r="E109" s="33"/>
+    </row>
+    <row r="110" spans="1:5">
+      <c r="A110" s="10"/>
+      <c r="B110" s="31"/>
+      <c r="C110" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="E110" s="6"/>
+      <c r="E110" s="33"/>
     </row>
     <row r="111" spans="1:5">
       <c r="A111" s="3"/>
-      <c r="B111" s="20" t="s">
+      <c r="B111" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="C111" s="18" t="s">
+      <c r="C111" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="E111" s="6" t="s">
+      <c r="E111" s="33" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="112" spans="1:5">
-      <c r="A112" s="7"/>
-      <c r="B112" s="9"/>
-      <c r="C112" s="10" t="s">
+      <c r="A112" s="6"/>
+      <c r="B112" s="30"/>
+      <c r="C112" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="E112" s="6"/>
+      <c r="E112" s="33"/>
     </row>
     <row r="113" spans="1:5">
-      <c r="A113" s="7"/>
-      <c r="B113" s="9"/>
-      <c r="C113" s="17" t="s">
+      <c r="A113" s="6"/>
+      <c r="B113" s="30"/>
+      <c r="C113" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="E113" s="6"/>
+      <c r="E113" s="33"/>
     </row>
     <row r="114" spans="1:5">
-      <c r="A114" s="7"/>
-      <c r="B114" s="9"/>
-      <c r="C114" s="17" t="s">
+      <c r="A114" s="6"/>
+      <c r="B114" s="30"/>
+      <c r="C114" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="E114" s="6"/>
+      <c r="E114" s="33"/>
     </row>
     <row r="115" spans="1:5">
-      <c r="A115" s="7"/>
-      <c r="B115" s="9"/>
-      <c r="C115" s="17" t="s">
+      <c r="A115" s="6"/>
+      <c r="B115" s="30"/>
+      <c r="C115" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="E115" s="6"/>
+      <c r="E115" s="33"/>
     </row>
     <row r="116" spans="1:5">
-      <c r="A116" s="7" t="s">
+      <c r="A116" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="B116" s="9"/>
-      <c r="C116" s="17" t="s">
+      <c r="B116" s="30"/>
+      <c r="C116" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="E116" s="6"/>
+      <c r="E116" s="33"/>
     </row>
     <row r="117" spans="1:5">
-      <c r="A117" s="7"/>
-      <c r="B117" s="9"/>
-      <c r="C117" s="17" t="s">
+      <c r="A117" s="6"/>
+      <c r="B117" s="30"/>
+      <c r="C117" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="E117" s="6"/>
+      <c r="E117" s="33"/>
     </row>
     <row r="118" spans="1:5">
-      <c r="A118" s="7"/>
-      <c r="B118" s="9"/>
-      <c r="C118" s="17" t="s">
+      <c r="A118" s="6"/>
+      <c r="B118" s="30"/>
+      <c r="C118" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="E118" s="6"/>
+      <c r="E118" s="33"/>
     </row>
     <row r="119" spans="1:5">
-      <c r="A119" s="7"/>
-      <c r="B119" s="9"/>
-      <c r="C119" s="17" t="s">
+      <c r="A119" s="6"/>
+      <c r="B119" s="30"/>
+      <c r="C119" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="E119" s="6"/>
+      <c r="E119" s="33"/>
     </row>
     <row r="120" spans="1:5">
-      <c r="A120" s="7"/>
-      <c r="B120" s="9"/>
-      <c r="C120" s="17" t="s">
+      <c r="A120" s="6"/>
+      <c r="B120" s="30"/>
+      <c r="C120" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="E120" s="6"/>
+      <c r="E120" s="33"/>
     </row>
     <row r="121" spans="1:5">
-      <c r="A121" s="7"/>
-      <c r="B121" s="9"/>
-      <c r="C121" s="17" t="s">
+      <c r="A121" s="6"/>
+      <c r="B121" s="30"/>
+      <c r="C121" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="E121" s="6"/>
+      <c r="E121" s="33"/>
     </row>
     <row r="122" spans="1:5">
-      <c r="A122" s="7"/>
-      <c r="B122" s="9"/>
-      <c r="C122" s="17" t="s">
+      <c r="A122" s="6"/>
+      <c r="B122" s="30"/>
+      <c r="C122" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="E122" s="6"/>
+      <c r="E122" s="33"/>
     </row>
     <row r="123" spans="1:5">
-      <c r="A123" s="7"/>
-      <c r="B123" s="9" t="s">
+      <c r="A123" s="6"/>
+      <c r="B123" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="C123" s="10" t="s">
+      <c r="C123" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="E123" s="6"/>
+      <c r="E123" s="33"/>
     </row>
     <row r="124" spans="1:5">
-      <c r="A124" s="7"/>
-      <c r="B124" s="9"/>
-      <c r="C124" s="17" t="s">
+      <c r="A124" s="6"/>
+      <c r="B124" s="30"/>
+      <c r="C124" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="E124" s="6"/>
+      <c r="E124" s="33"/>
     </row>
     <row r="125" spans="1:5">
-      <c r="A125" s="7"/>
-      <c r="B125" s="9"/>
-      <c r="C125" s="17" t="s">
+      <c r="A125" s="6"/>
+      <c r="B125" s="30"/>
+      <c r="C125" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="E125" s="6"/>
+      <c r="E125" s="33"/>
     </row>
     <row r="126" spans="1:5">
-      <c r="A126" s="7"/>
-      <c r="B126" s="9"/>
-      <c r="C126" s="17" t="s">
+      <c r="A126" s="6"/>
+      <c r="B126" s="30"/>
+      <c r="C126" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="E126" s="6"/>
+      <c r="E126" s="33"/>
     </row>
     <row r="127" spans="1:5">
-      <c r="A127" s="7" t="s">
+      <c r="A127" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="B127" s="9"/>
-      <c r="C127" s="17" t="s">
+      <c r="B127" s="30"/>
+      <c r="C127" s="14" t="s">
         <v>136</v>
       </c>
-      <c r="E127" s="6"/>
+      <c r="E127" s="33"/>
     </row>
     <row r="128" spans="1:5">
-      <c r="A128" s="7"/>
-      <c r="B128" s="9"/>
-      <c r="C128" s="17" t="s">
+      <c r="A128" s="6"/>
+      <c r="B128" s="30"/>
+      <c r="C128" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="E128" s="6"/>
+      <c r="E128" s="33"/>
     </row>
     <row r="129" spans="1:5">
-      <c r="A129" s="7"/>
-      <c r="B129" s="9"/>
-      <c r="C129" s="17" t="s">
+      <c r="A129" s="6"/>
+      <c r="B129" s="30"/>
+      <c r="C129" s="14" t="s">
         <v>138</v>
       </c>
-      <c r="E129" s="6"/>
+      <c r="E129" s="33"/>
     </row>
     <row r="130" spans="1:5">
-      <c r="A130" s="7"/>
-      <c r="B130" s="9"/>
-      <c r="C130" s="17" t="s">
+      <c r="A130" s="6"/>
+      <c r="B130" s="30"/>
+      <c r="C130" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="E130" s="6"/>
+      <c r="E130" s="33"/>
     </row>
     <row r="131" spans="1:5">
-      <c r="A131" s="7"/>
-      <c r="B131" s="9"/>
-      <c r="C131" s="17" t="s">
+      <c r="A131" s="6"/>
+      <c r="B131" s="30"/>
+      <c r="C131" s="14" t="s">
         <v>140</v>
       </c>
-      <c r="E131" s="6"/>
+      <c r="E131" s="33"/>
     </row>
     <row r="132" spans="1:5">
-      <c r="A132" s="7"/>
-      <c r="B132" s="9"/>
-      <c r="C132" s="17" t="s">
+      <c r="A132" s="6"/>
+      <c r="B132" s="30"/>
+      <c r="C132" s="14" t="s">
         <v>141</v>
       </c>
-      <c r="E132" s="6"/>
-    </row>
-    <row r="133" ht="27" spans="1:5">
-      <c r="A133" s="12"/>
-      <c r="B133" s="13"/>
-      <c r="C133" s="17" t="s">
+      <c r="E132" s="33"/>
+    </row>
+    <row r="133" spans="1:5">
+      <c r="A133" s="10"/>
+      <c r="B133" s="31"/>
+      <c r="C133" s="14" t="s">
         <v>142</v>
       </c>
-      <c r="E133" s="6"/>
+      <c r="E133" s="33"/>
     </row>
     <row r="134" spans="1:5">
       <c r="A134" s="3"/>
       <c r="B134" s="4"/>
-      <c r="C134" s="15" t="s">
+      <c r="C134" s="12" t="s">
         <v>143</v>
       </c>
-      <c r="E134" s="6"/>
+      <c r="E134" s="33"/>
     </row>
     <row r="135" spans="1:5">
-      <c r="A135" s="7"/>
-      <c r="B135" s="9" t="s">
+      <c r="A135" s="6"/>
+      <c r="B135" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="C135" s="17" t="s">
+      <c r="C135" s="14" t="s">
         <v>144</v>
       </c>
-      <c r="E135" s="6"/>
+      <c r="E135" s="33"/>
     </row>
     <row r="136" spans="1:5">
-      <c r="A136" s="7"/>
-      <c r="B136" s="9"/>
-      <c r="C136" s="17" t="s">
+      <c r="A136" s="6"/>
+      <c r="B136" s="30"/>
+      <c r="C136" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="E136" s="6"/>
+      <c r="E136" s="33"/>
     </row>
     <row r="137" spans="1:5">
-      <c r="A137" s="7"/>
-      <c r="B137" s="9"/>
-      <c r="C137" s="17" t="s">
+      <c r="A137" s="6"/>
+      <c r="B137" s="30"/>
+      <c r="C137" s="14" t="s">
         <v>146</v>
       </c>
-      <c r="E137" s="6"/>
+      <c r="E137" s="33"/>
     </row>
     <row r="138" spans="1:5">
-      <c r="A138" s="7"/>
-      <c r="B138" s="9"/>
-      <c r="C138" s="17" t="s">
+      <c r="A138" s="6"/>
+      <c r="B138" s="30"/>
+      <c r="C138" s="14" t="s">
         <v>147</v>
       </c>
-      <c r="E138" s="6"/>
+      <c r="E138" s="33"/>
     </row>
     <row r="139" spans="1:5">
-      <c r="A139" s="7"/>
-      <c r="B139" s="9"/>
-      <c r="C139" s="17" t="s">
+      <c r="A139" s="6"/>
+      <c r="B139" s="30"/>
+      <c r="C139" s="14" t="s">
         <v>148</v>
       </c>
-      <c r="E139" s="6"/>
+      <c r="E139" s="33"/>
     </row>
     <row r="140" spans="1:5">
-      <c r="A140" s="7"/>
-      <c r="B140" s="9"/>
-      <c r="C140" s="17" t="s">
+      <c r="A140" s="6"/>
+      <c r="B140" s="30"/>
+      <c r="C140" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="E140" s="6"/>
+      <c r="E140" s="33"/>
     </row>
     <row r="141" spans="1:5">
-      <c r="A141" s="7"/>
-      <c r="B141" s="9"/>
-      <c r="C141" s="17" t="s">
+      <c r="A141" s="6"/>
+      <c r="B141" s="30"/>
+      <c r="C141" s="14" t="s">
         <v>150</v>
       </c>
-      <c r="E141" s="6"/>
+      <c r="E141" s="33"/>
     </row>
     <row r="142" spans="1:5">
-      <c r="A142" s="7" t="s">
+      <c r="A142" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="B142" s="9"/>
-      <c r="C142" s="17" t="s">
+      <c r="B142" s="30"/>
+      <c r="C142" s="14" t="s">
         <v>152</v>
       </c>
-      <c r="E142" s="6"/>
+      <c r="E142" s="33"/>
     </row>
     <row r="143" spans="1:5">
-      <c r="A143" s="7"/>
-      <c r="B143" s="9"/>
-      <c r="C143" s="17" t="s">
+      <c r="A143" s="6"/>
+      <c r="B143" s="30"/>
+      <c r="C143" s="14" t="s">
         <v>153</v>
       </c>
-      <c r="E143" s="6"/>
+      <c r="E143" s="33"/>
     </row>
     <row r="144" spans="1:5">
-      <c r="A144" s="7"/>
-      <c r="B144" s="9"/>
-      <c r="C144" s="17" t="s">
+      <c r="A144" s="6"/>
+      <c r="B144" s="30"/>
+      <c r="C144" s="14" t="s">
         <v>154</v>
       </c>
-      <c r="E144" s="6"/>
-    </row>
-    <row r="145" ht="52.5" spans="1:5">
-      <c r="A145" s="7"/>
-      <c r="B145" s="9"/>
-      <c r="C145" s="23" t="s">
+      <c r="E144" s="33"/>
+    </row>
+    <row r="145" spans="1:5" ht="51.6">
+      <c r="A145" s="6"/>
+      <c r="B145" s="30"/>
+      <c r="C145" s="19" t="s">
         <v>155</v>
       </c>
-      <c r="E145" s="6"/>
+      <c r="E145" s="33"/>
     </row>
     <row r="146" spans="1:5">
-      <c r="A146" s="7"/>
-      <c r="B146" s="9"/>
-      <c r="C146" s="17" t="s">
+      <c r="A146" s="6"/>
+      <c r="B146" s="30"/>
+      <c r="C146" s="14" t="s">
         <v>156</v>
       </c>
-      <c r="E146" s="6"/>
+      <c r="E146" s="33"/>
     </row>
     <row r="147" spans="1:5">
-      <c r="A147" s="7"/>
-      <c r="B147" s="9"/>
-      <c r="C147" s="17" t="s">
+      <c r="A147" s="6"/>
+      <c r="B147" s="30"/>
+      <c r="C147" s="14" t="s">
         <v>157</v>
       </c>
-      <c r="E147" s="6"/>
+      <c r="E147" s="33"/>
     </row>
     <row r="148" spans="1:5">
-      <c r="A148" s="7"/>
-      <c r="B148" s="9"/>
-      <c r="C148" s="17" t="s">
+      <c r="A148" s="6"/>
+      <c r="B148" s="30"/>
+      <c r="C148" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="E148" s="6"/>
+      <c r="E148" s="33"/>
     </row>
     <row r="149" spans="1:5">
-      <c r="A149" s="7"/>
-      <c r="B149" s="9"/>
-      <c r="C149" s="17" t="s">
+      <c r="A149" s="6"/>
+      <c r="B149" s="30"/>
+      <c r="C149" s="14" t="s">
         <v>159</v>
       </c>
-      <c r="E149" s="6"/>
+      <c r="E149" s="33"/>
     </row>
     <row r="150" spans="1:5">
-      <c r="A150" s="7"/>
-      <c r="B150" s="9"/>
-      <c r="C150" s="17" t="s">
+      <c r="A150" s="6"/>
+      <c r="B150" s="30"/>
+      <c r="C150" s="14" t="s">
         <v>160</v>
       </c>
-      <c r="E150" s="6"/>
+      <c r="E150" s="33"/>
     </row>
     <row r="151" spans="1:5">
-      <c r="A151" s="7"/>
-      <c r="B151" s="9"/>
-      <c r="C151" s="17" t="s">
+      <c r="A151" s="6"/>
+      <c r="B151" s="30"/>
+      <c r="C151" s="14" t="s">
         <v>161</v>
       </c>
-      <c r="E151" s="6"/>
-    </row>
-    <row r="152" ht="27" spans="1:5">
-      <c r="A152" s="12"/>
-      <c r="B152" s="13"/>
-      <c r="C152" s="17" t="s">
+      <c r="E151" s="33"/>
+    </row>
+    <row r="152" spans="1:5">
+      <c r="A152" s="10"/>
+      <c r="B152" s="31"/>
+      <c r="C152" s="14" t="s">
         <v>162</v>
       </c>
-      <c r="E152" s="6"/>
+      <c r="E152" s="33"/>
     </row>
     <row r="153" spans="1:5">
       <c r="A153" s="3"/>
       <c r="B153" s="4"/>
-      <c r="C153" s="15" t="s">
+      <c r="C153" s="12" t="s">
         <v>163</v>
       </c>
-      <c r="E153" s="6"/>
+      <c r="E153" s="33"/>
     </row>
     <row r="154" spans="1:5">
-      <c r="A154" s="7"/>
-      <c r="B154" s="9" t="s">
+      <c r="A154" s="6"/>
+      <c r="B154" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="C154" s="24" t="s">
+      <c r="C154" s="17" t="s">
         <v>164</v>
       </c>
-      <c r="E154" s="6"/>
+      <c r="E154" s="33"/>
     </row>
     <row r="155" spans="1:5">
-      <c r="A155" s="7"/>
-      <c r="B155" s="9"/>
-      <c r="C155" s="24" t="s">
+      <c r="A155" s="6"/>
+      <c r="B155" s="30"/>
+      <c r="C155" s="17" t="s">
         <v>165</v>
       </c>
-      <c r="E155" s="6"/>
+      <c r="E155" s="33"/>
     </row>
     <row r="156" spans="1:5">
-      <c r="A156" s="7"/>
-      <c r="B156" s="9"/>
-      <c r="C156" s="24" t="s">
+      <c r="A156" s="6"/>
+      <c r="B156" s="30"/>
+      <c r="C156" s="17" t="s">
         <v>166</v>
       </c>
-      <c r="E156" s="6"/>
+      <c r="E156" s="33"/>
     </row>
     <row r="157" spans="1:5">
-      <c r="A157" s="7"/>
-      <c r="B157" s="9"/>
-      <c r="C157" s="24" t="s">
+      <c r="A157" s="6"/>
+      <c r="B157" s="30"/>
+      <c r="C157" s="17" t="s">
         <v>167</v>
       </c>
-      <c r="E157" s="6"/>
+      <c r="E157" s="33"/>
     </row>
     <row r="158" spans="1:5">
-      <c r="A158" s="7"/>
-      <c r="B158" s="9"/>
-      <c r="C158" s="24" t="s">
+      <c r="A158" s="6"/>
+      <c r="B158" s="30"/>
+      <c r="C158" s="17" t="s">
         <v>168</v>
       </c>
-      <c r="E158" s="6"/>
+      <c r="E158" s="33"/>
     </row>
     <row r="159" spans="1:5">
-      <c r="A159" s="7" t="s">
+      <c r="A159" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="B159" s="9"/>
-      <c r="C159" s="24" t="s">
+      <c r="B159" s="30"/>
+      <c r="C159" s="20" t="s">
         <v>170</v>
       </c>
-      <c r="E159" s="6"/>
+      <c r="E159" s="33"/>
     </row>
     <row r="160" spans="1:5">
-      <c r="A160" s="7"/>
-      <c r="B160" s="9"/>
-      <c r="C160" s="24" t="s">
+      <c r="A160" s="6"/>
+      <c r="B160" s="30"/>
+      <c r="C160" s="20" t="s">
         <v>171</v>
       </c>
-      <c r="E160" s="6"/>
-    </row>
-    <row r="161" ht="52.5" spans="1:5">
-      <c r="A161" s="7"/>
-      <c r="B161" s="9"/>
-      <c r="C161" s="25" t="s">
+      <c r="E160" s="33"/>
+    </row>
+    <row r="161" spans="1:5" ht="51.6">
+      <c r="A161" s="6"/>
+      <c r="B161" s="30"/>
+      <c r="C161" s="21" t="s">
         <v>172</v>
       </c>
-      <c r="E161" s="6"/>
+      <c r="E161" s="33"/>
     </row>
     <row r="162" spans="1:5">
-      <c r="A162" s="7"/>
-      <c r="B162" s="9"/>
-      <c r="C162" s="24" t="s">
+      <c r="A162" s="6"/>
+      <c r="B162" s="30"/>
+      <c r="C162" s="20" t="s">
         <v>173</v>
       </c>
-      <c r="E162" s="6"/>
+      <c r="E162" s="33"/>
     </row>
     <row r="163" spans="1:5">
-      <c r="A163" s="7"/>
-      <c r="B163" s="9"/>
-      <c r="C163" s="24" t="s">
+      <c r="A163" s="6"/>
+      <c r="B163" s="30"/>
+      <c r="C163" s="20" t="s">
         <v>174</v>
       </c>
-      <c r="E163" s="6"/>
+      <c r="E163" s="33"/>
     </row>
     <row r="164" spans="1:5">
-      <c r="A164" s="7"/>
-      <c r="B164" s="9"/>
-      <c r="C164" s="24" t="s">
+      <c r="A164" s="6"/>
+      <c r="B164" s="30"/>
+      <c r="C164" s="20" t="s">
         <v>175</v>
       </c>
-      <c r="E164" s="6"/>
+      <c r="E164" s="33"/>
     </row>
     <row r="165" spans="1:5">
-      <c r="A165" s="7"/>
-      <c r="B165" s="9"/>
-      <c r="C165" s="26" t="s">
+      <c r="A165" s="6"/>
+      <c r="B165" s="30"/>
+      <c r="C165" s="22" t="s">
         <v>176</v>
       </c>
-      <c r="E165" s="6"/>
+      <c r="E165" s="33"/>
     </row>
     <row r="166" spans="1:5">
-      <c r="A166" s="7"/>
-      <c r="B166" s="9"/>
-      <c r="C166" s="26" t="s">
+      <c r="A166" s="6"/>
+      <c r="B166" s="30"/>
+      <c r="C166" s="22" t="s">
         <v>177</v>
       </c>
-      <c r="E166" s="6"/>
+      <c r="E166" s="33"/>
     </row>
     <row r="167" spans="1:5">
-      <c r="A167" s="7"/>
-      <c r="B167" s="9"/>
-      <c r="C167" s="26" t="s">
+      <c r="A167" s="6"/>
+      <c r="B167" s="30"/>
+      <c r="C167" s="22" t="s">
         <v>178</v>
       </c>
-      <c r="E167" s="6"/>
+      <c r="E167" s="33"/>
     </row>
     <row r="168" spans="1:5">
-      <c r="A168" s="7"/>
-      <c r="B168" s="9"/>
-      <c r="C168" s="26" t="s">
+      <c r="A168" s="6"/>
+      <c r="B168" s="30"/>
+      <c r="C168" s="22" t="s">
         <v>179</v>
       </c>
-      <c r="E168" s="6"/>
+      <c r="E168" s="33"/>
     </row>
     <row r="169" spans="1:5">
-      <c r="A169" s="7"/>
-      <c r="B169" s="9"/>
-      <c r="C169" s="26" t="s">
+      <c r="A169" s="6"/>
+      <c r="B169" s="30"/>
+      <c r="C169" s="22" t="s">
         <v>180</v>
       </c>
-      <c r="E169" s="6"/>
+      <c r="E169" s="33"/>
     </row>
     <row r="170" spans="1:5">
-      <c r="A170" s="7"/>
-      <c r="B170" s="9"/>
-      <c r="C170" s="26"/>
-      <c r="E170" s="6"/>
+      <c r="A170" s="6"/>
+      <c r="B170" s="30"/>
+      <c r="C170" s="22"/>
+      <c r="E170" s="33"/>
     </row>
     <row r="171" spans="1:5">
-      <c r="A171" s="7"/>
-      <c r="B171" s="9"/>
-      <c r="C171" s="26" t="s">
+      <c r="A171" s="6"/>
+      <c r="B171" s="30"/>
+      <c r="C171" s="35" t="s">
         <v>181</v>
       </c>
-      <c r="E171" s="6"/>
-    </row>
-    <row r="172" ht="27" spans="1:5">
-      <c r="A172" s="12"/>
-      <c r="B172" s="13"/>
-      <c r="C172" s="27" t="s">
+      <c r="E171" s="33"/>
+    </row>
+    <row r="172" spans="1:5">
+      <c r="A172" s="10"/>
+      <c r="B172" s="31"/>
+      <c r="C172" s="23" t="s">
         <v>182</v>
       </c>
-      <c r="E172" s="6"/>
+      <c r="E172" s="33"/>
     </row>
     <row r="173" spans="1:5">
       <c r="A173" s="3"/>
       <c r="B173" s="4"/>
-      <c r="C173" s="18" t="s">
+      <c r="C173" s="15" t="s">
         <v>183</v>
       </c>
-      <c r="E173" s="28" t="s">
+      <c r="E173" s="34" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="174" spans="1:5">
-      <c r="A174" s="7"/>
-      <c r="B174" s="9" t="s">
+      <c r="A174" s="6"/>
+      <c r="B174" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="C174" s="10" t="s">
+      <c r="C174" s="8" t="s">
         <v>185</v>
       </c>
-      <c r="E174" s="28"/>
+      <c r="E174" s="34"/>
     </row>
     <row r="175" spans="1:5">
-      <c r="A175" s="7"/>
-      <c r="B175" s="9"/>
-      <c r="C175" s="24" t="s">
+      <c r="A175" s="6"/>
+      <c r="B175" s="30"/>
+      <c r="C175" s="20" t="s">
         <v>186</v>
       </c>
-      <c r="E175" s="28"/>
+      <c r="E175" s="34"/>
     </row>
     <row r="176" spans="1:5">
-      <c r="A176" s="7"/>
-      <c r="B176" s="9"/>
-      <c r="C176" s="24" t="s">
+      <c r="A176" s="6"/>
+      <c r="B176" s="30"/>
+      <c r="C176" s="20" t="s">
         <v>187</v>
       </c>
-      <c r="E176" s="28"/>
+      <c r="E176" s="34"/>
     </row>
     <row r="177" spans="1:5">
-      <c r="A177" s="7"/>
-      <c r="B177" s="9"/>
-      <c r="C177" s="24" t="s">
+      <c r="A177" s="6"/>
+      <c r="B177" s="30"/>
+      <c r="C177" s="20" t="s">
         <v>188</v>
       </c>
-      <c r="E177" s="28"/>
+      <c r="E177" s="34"/>
     </row>
     <row r="178" spans="1:5">
-      <c r="A178" s="7"/>
-      <c r="B178" s="9"/>
-      <c r="C178" s="24" t="s">
+      <c r="A178" s="6"/>
+      <c r="B178" s="30"/>
+      <c r="C178" s="20" t="s">
         <v>189</v>
       </c>
-      <c r="E178" s="28"/>
+      <c r="E178" s="34"/>
     </row>
     <row r="179" spans="1:5">
-      <c r="A179" s="7" t="s">
+      <c r="A179" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="B179" s="9"/>
-      <c r="C179" s="24" t="s">
+      <c r="B179" s="30"/>
+      <c r="C179" s="20" t="s">
         <v>191</v>
       </c>
-      <c r="E179" s="28"/>
+      <c r="E179" s="34"/>
     </row>
     <row r="180" spans="1:5">
-      <c r="A180" s="7"/>
-      <c r="B180" s="9"/>
-      <c r="C180" s="24" t="s">
+      <c r="A180" s="6"/>
+      <c r="B180" s="30"/>
+      <c r="C180" s="20" t="s">
         <v>192</v>
       </c>
-      <c r="E180" s="28"/>
+      <c r="E180" s="34"/>
     </row>
     <row r="181" spans="1:5">
-      <c r="A181" s="7"/>
-      <c r="B181" s="9"/>
-      <c r="C181" s="10" t="s">
+      <c r="A181" s="6"/>
+      <c r="B181" s="30"/>
+      <c r="C181" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="E181" s="28"/>
+      <c r="E181" s="34"/>
     </row>
     <row r="182" spans="1:5">
-      <c r="A182" s="7"/>
-      <c r="B182" s="9"/>
-      <c r="C182" s="24" t="s">
+      <c r="A182" s="6"/>
+      <c r="B182" s="30"/>
+      <c r="C182" s="20" t="s">
         <v>194</v>
       </c>
-      <c r="E182" s="28"/>
-    </row>
-    <row r="183" ht="78.75" spans="1:5">
-      <c r="A183" s="7"/>
-      <c r="B183" s="9"/>
-      <c r="C183" s="25" t="s">
+      <c r="E182" s="34"/>
+    </row>
+    <row r="183" spans="1:5" ht="51.6">
+      <c r="A183" s="6"/>
+      <c r="B183" s="30"/>
+      <c r="C183" s="21" t="s">
         <v>195</v>
       </c>
-      <c r="E183" s="28"/>
+      <c r="E183" s="34"/>
     </row>
     <row r="184" spans="1:5">
-      <c r="A184" s="7"/>
-      <c r="B184" s="9"/>
-      <c r="C184" s="24" t="s">
+      <c r="A184" s="6"/>
+      <c r="B184" s="30"/>
+      <c r="C184" s="20" t="s">
         <v>196</v>
       </c>
-      <c r="E184" s="28"/>
+      <c r="E184" s="34"/>
     </row>
     <row r="185" spans="1:5">
-      <c r="A185" s="7"/>
-      <c r="B185" s="9"/>
-      <c r="C185" s="24" t="s">
+      <c r="A185" s="6"/>
+      <c r="B185" s="30"/>
+      <c r="C185" s="20" t="s">
         <v>197</v>
       </c>
-      <c r="E185" s="28"/>
+      <c r="E185" s="34"/>
     </row>
     <row r="186" spans="1:5">
-      <c r="A186" s="7"/>
-      <c r="B186" s="9" t="s">
+      <c r="A186" s="6"/>
+      <c r="B186" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="C186" s="29" t="s">
+      <c r="C186" s="25" t="s">
         <v>198</v>
       </c>
-      <c r="E186" s="28"/>
+      <c r="E186" s="34"/>
     </row>
     <row r="187" spans="1:5">
-      <c r="A187" s="7"/>
-      <c r="B187" s="9"/>
-      <c r="C187" s="30" t="s">
+      <c r="A187" s="6"/>
+      <c r="B187" s="30"/>
+      <c r="C187" s="26" t="s">
         <v>199</v>
       </c>
-      <c r="E187" s="28"/>
+      <c r="E187" s="34"/>
     </row>
     <row r="188" spans="1:5">
-      <c r="A188" s="7"/>
-      <c r="B188" s="9"/>
-      <c r="C188" s="30" t="s">
+      <c r="A188" s="6"/>
+      <c r="B188" s="30"/>
+      <c r="C188" s="26" t="s">
         <v>200</v>
       </c>
-      <c r="E188" s="28"/>
+      <c r="E188" s="34"/>
     </row>
     <row r="189" spans="1:5">
-      <c r="A189" s="7"/>
-      <c r="B189" s="9"/>
-      <c r="C189" s="31" t="s">
+      <c r="A189" s="6"/>
+      <c r="B189" s="30"/>
+      <c r="C189" s="27" t="s">
         <v>201</v>
       </c>
-      <c r="E189" s="28"/>
-    </row>
-    <row r="190" ht="51" spans="1:5">
-      <c r="A190" s="7" t="s">
+      <c r="E189" s="34"/>
+    </row>
+    <row r="190" spans="1:5" ht="49.2">
+      <c r="A190" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="B190" s="9"/>
-      <c r="C190" s="31" t="s">
+      <c r="B190" s="30"/>
+      <c r="C190" s="27" t="s">
         <v>203</v>
       </c>
-      <c r="E190" s="28"/>
+      <c r="E190" s="34"/>
     </row>
     <row r="191" spans="1:5">
-      <c r="A191" s="7"/>
-      <c r="B191" s="9"/>
-      <c r="C191" s="31" t="s">
+      <c r="A191" s="6"/>
+      <c r="B191" s="30"/>
+      <c r="C191" s="27" t="s">
         <v>204</v>
       </c>
-      <c r="E191" s="28"/>
+      <c r="E191" s="34"/>
     </row>
     <row r="192" spans="1:5">
-      <c r="A192" s="7"/>
-      <c r="B192" s="9"/>
-      <c r="C192" s="31" t="s">
+      <c r="A192" s="6"/>
+      <c r="B192" s="30"/>
+      <c r="C192" s="27" t="s">
         <v>205</v>
       </c>
-      <c r="E192" s="28"/>
+      <c r="E192" s="34"/>
     </row>
     <row r="193" spans="1:5">
-      <c r="A193" s="7"/>
-      <c r="B193" s="9"/>
-      <c r="C193" s="31" t="s">
+      <c r="A193" s="6"/>
+      <c r="B193" s="30"/>
+      <c r="C193" s="27" t="s">
         <v>206</v>
       </c>
-      <c r="E193" s="28"/>
+      <c r="E193" s="34"/>
     </row>
     <row r="194" spans="1:5">
-      <c r="A194" s="7"/>
-      <c r="B194" s="9"/>
-      <c r="C194" s="31" t="s">
+      <c r="A194" s="6"/>
+      <c r="B194" s="30"/>
+      <c r="C194" s="27" t="s">
         <v>207</v>
       </c>
-      <c r="E194" s="28"/>
+      <c r="E194" s="34"/>
     </row>
     <row r="195" spans="1:5">
-      <c r="A195" s="7"/>
-      <c r="B195" s="9"/>
-      <c r="C195" s="31" t="s">
+      <c r="A195" s="6"/>
+      <c r="B195" s="30"/>
+      <c r="C195" s="27" t="s">
         <v>208</v>
       </c>
-      <c r="E195" s="28"/>
+      <c r="E195" s="34"/>
     </row>
     <row r="196" spans="1:5">
-      <c r="A196" s="7"/>
-      <c r="B196" s="9" t="s">
+      <c r="A196" s="6"/>
+      <c r="B196" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="C196" s="29" t="s">
+      <c r="C196" s="25" t="s">
         <v>209</v>
       </c>
-      <c r="E196" s="28"/>
+      <c r="E196" s="34"/>
     </row>
     <row r="197" spans="1:5">
-      <c r="A197" s="7"/>
-      <c r="B197" s="9"/>
-      <c r="C197" s="32" t="s">
+      <c r="A197" s="6"/>
+      <c r="B197" s="30"/>
+      <c r="C197" s="28" t="s">
         <v>210</v>
       </c>
-      <c r="E197" s="28"/>
+      <c r="E197" s="34"/>
     </row>
     <row r="198" spans="1:5">
-      <c r="A198" s="7"/>
-      <c r="B198" s="9"/>
-      <c r="C198" s="29" t="s">
+      <c r="A198" s="6"/>
+      <c r="B198" s="30"/>
+      <c r="C198" s="25" t="s">
         <v>211</v>
       </c>
-      <c r="E198" s="28"/>
+      <c r="E198" s="34"/>
     </row>
     <row r="199" spans="1:5">
-      <c r="A199" s="7" t="s">
+      <c r="A199" s="6" t="s">
         <v>212</v>
       </c>
-      <c r="B199" s="9"/>
-      <c r="C199" s="32" t="s">
+      <c r="B199" s="30"/>
+      <c r="C199" s="28" t="s">
         <v>213</v>
       </c>
-      <c r="E199" s="28"/>
-    </row>
-    <row r="200" spans="2:5">
-      <c r="B200" s="9"/>
-      <c r="C200" s="33" t="s">
+      <c r="E199" s="34"/>
+    </row>
+    <row r="200" spans="1:5">
+      <c r="B200" s="30"/>
+      <c r="C200" s="29" t="s">
         <v>214</v>
       </c>
-      <c r="E200" s="28"/>
+      <c r="E200" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="E173:E199"/>
+    <mergeCell ref="E3:E15"/>
+    <mergeCell ref="E16:E37"/>
+    <mergeCell ref="E38:E57"/>
+    <mergeCell ref="E58:E110"/>
+    <mergeCell ref="E111:E172"/>
+    <mergeCell ref="B135:B152"/>
+    <mergeCell ref="B154:B172"/>
+    <mergeCell ref="B174:B185"/>
+    <mergeCell ref="B186:B195"/>
+    <mergeCell ref="B196:B200"/>
+    <mergeCell ref="B80:B92"/>
+    <mergeCell ref="B93:B101"/>
+    <mergeCell ref="B102:B110"/>
+    <mergeCell ref="B111:B122"/>
+    <mergeCell ref="B123:B133"/>
     <mergeCell ref="B5:B15"/>
     <mergeCell ref="B17:B37"/>
     <mergeCell ref="B39:B43"/>
     <mergeCell ref="B45:B57"/>
     <mergeCell ref="B59:B79"/>
-    <mergeCell ref="B80:B92"/>
-    <mergeCell ref="B93:B101"/>
-    <mergeCell ref="B102:B110"/>
-    <mergeCell ref="B111:B122"/>
-    <mergeCell ref="B123:B133"/>
-    <mergeCell ref="B135:B152"/>
-    <mergeCell ref="B154:B172"/>
-    <mergeCell ref="B174:B185"/>
-    <mergeCell ref="B186:B195"/>
-    <mergeCell ref="B196:B200"/>
-    <mergeCell ref="E3:E15"/>
-    <mergeCell ref="E16:E37"/>
-    <mergeCell ref="E38:E57"/>
-    <mergeCell ref="E58:E110"/>
-    <mergeCell ref="E111:E172"/>
-    <mergeCell ref="E173:E199"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>